<commit_message>
Fix IEA energy balance: correct negative/positive balance Issues. Process IEA energy production data as non combustion/process activity data rather than combustion activity data. Change activity_input_mapping from xlsx to csv file.
</commit_message>
<xml_diff>
--- a/input/mappings/Master_Fuel_Sector_List.xlsx
+++ b/input/mappings/Master_Fuel_Sector_List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="1260" windowWidth="21840" windowHeight="13335" tabRatio="500"/>
+    <workbookView xWindow="24240" yWindow="3680" windowWidth="12340" windowHeight="15220" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sectors" sheetId="1" r:id="rId1"/>
     <sheet name="Fuels" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="89">
   <si>
     <t>sector</t>
   </si>
@@ -284,13 +284,16 @@
   </si>
   <si>
     <t>energytrans_petr_refin</t>
+  </si>
+  <si>
+    <t>TJ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -315,7 +318,12 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Times"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -335,7 +343,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="97">
+  <cellStyleXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -433,12 +441,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="97">
+  <cellStyles count="103">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -487,6 +502,9 @@
     <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -535,6 +553,9 @@
     <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -869,400 +890,481 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="24.75" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>81</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" ht="15">
+      <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" ht="15">
+      <c r="A3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" ht="15">
+      <c r="A4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" ht="15">
+      <c r="A5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" ht="15">
+      <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" ht="15">
+      <c r="A7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" ht="15">
+      <c r="A8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" ht="15">
+      <c r="A9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" ht="15">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" ht="15">
+      <c r="A11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" ht="15">
+      <c r="A12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" ht="15">
+      <c r="A13" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" ht="15">
+      <c r="A14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" ht="15">
+      <c r="A15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" ht="15">
+      <c r="A16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" ht="15">
+      <c r="A17" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" ht="15">
+      <c r="A18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" ht="15">
+      <c r="A19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" ht="15">
+      <c r="A20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" ht="15">
+      <c r="A21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" ht="15">
+      <c r="A22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" ht="15">
+      <c r="A23" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" ht="15">
+      <c r="A24" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C24" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="D24" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" ht="15">
+      <c r="A25" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" ht="15">
+      <c r="A26" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C26" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="D26" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" ht="15">
+      <c r="A27" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C27" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7" t="s">
-        <v>84</v>
-      </c>
-      <c r="D7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C9" t="s">
-        <v>84</v>
-      </c>
-      <c r="D9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" t="s">
-        <v>72</v>
-      </c>
-      <c r="C11" t="s">
-        <v>84</v>
-      </c>
-      <c r="D11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>72</v>
-      </c>
-      <c r="C12" t="s">
-        <v>84</v>
-      </c>
-      <c r="D12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>87</v>
-      </c>
-      <c r="B13" t="s">
-        <v>72</v>
-      </c>
-      <c r="C13" t="s">
-        <v>84</v>
-      </c>
-      <c r="D13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" t="s">
-        <v>72</v>
-      </c>
-      <c r="C14" t="s">
-        <v>84</v>
-      </c>
-      <c r="D14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" t="s">
-        <v>72</v>
-      </c>
-      <c r="C15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" t="s">
-        <v>72</v>
-      </c>
-      <c r="C16" t="s">
-        <v>84</v>
-      </c>
-      <c r="D16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>73</v>
-      </c>
-      <c r="B17" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C18" t="s">
-        <v>84</v>
-      </c>
-      <c r="D18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" t="s">
-        <v>72</v>
-      </c>
-      <c r="C19" t="s">
-        <v>84</v>
-      </c>
-      <c r="D19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" t="s">
-        <v>72</v>
-      </c>
-      <c r="C20" t="s">
-        <v>84</v>
-      </c>
-      <c r="D20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" t="s">
-        <v>72</v>
-      </c>
-      <c r="C21" t="s">
-        <v>84</v>
-      </c>
-      <c r="D21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" t="s">
-        <v>72</v>
-      </c>
-      <c r="C22" t="s">
-        <v>84</v>
-      </c>
-      <c r="D22" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" t="s">
-        <v>74</v>
-      </c>
-      <c r="C23" t="s">
-        <v>84</v>
-      </c>
-      <c r="D23" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24" t="s">
-        <v>71</v>
-      </c>
-      <c r="C24" t="s">
-        <v>82</v>
-      </c>
-      <c r="D24" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" t="s">
-        <v>76</v>
-      </c>
-      <c r="C25" t="s">
-        <v>83</v>
-      </c>
-      <c r="D25" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" t="s">
-        <v>71</v>
-      </c>
-      <c r="C26" t="s">
-        <v>82</v>
-      </c>
-      <c r="D26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" t="s">
-        <v>71</v>
-      </c>
-      <c r="C27" t="s">
-        <v>82</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="D27" s="2" t="s">
         <v>49</v>
       </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1273,19 +1375,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="19.625" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15">
       <c r="A1" s="1" t="s">
         <v>50</v>
       </c>
@@ -1298,136 +1400,146 @@
       <c r="D1" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" ht="15">
+      <c r="A2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" ht="15">
+      <c r="A3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" ht="15">
+      <c r="A4" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" ht="15">
+      <c r="A5" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" ht="15">
+      <c r="A6" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" ht="15">
+      <c r="A7" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" ht="15">
+      <c r="A8" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" ht="15">
+      <c r="A9" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" ht="15">
+      <c r="A10" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>86</v>
       </c>
+      <c r="E10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Fixes energy as driver data and it's incorporation into NC_activity data bases
</commit_message>
<xml_diff>
--- a/input/mappings/Master_Fuel_Sector_List.xlsx
+++ b/input/mappings/Master_Fuel_Sector_List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="24240" yWindow="3680" windowWidth="12340" windowHeight="15220" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="24240" yWindow="3680" windowWidth="12340" windowHeight="15220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sectors" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="90">
   <si>
     <t>sector</t>
   </si>
@@ -287,6 +287,9 @@
   </si>
   <si>
     <t>TJ</t>
+  </si>
+  <si>
+    <t>crude_oil</t>
   </si>
 </sst>
 </file>
@@ -892,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -959,7 +962,7 @@
         <v>22</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>22</v>
+        <v>89</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>84</v>
@@ -1377,7 +1380,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixes coke oven process data. adds mapping files and documentation.
</commit_message>
<xml_diff>
--- a/input/mappings/Master_Fuel_Sector_List.xlsx
+++ b/input/mappings/Master_Fuel_Sector_List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="24240" yWindow="3680" windowWidth="12340" windowHeight="15220" tabRatio="500"/>
+    <workbookView xWindow="24900" yWindow="160" windowWidth="15540" windowHeight="15020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sectors" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="91">
   <si>
     <t>sector</t>
   </si>
@@ -290,6 +290,9 @@
   </si>
   <si>
     <t>crude_oil</t>
+  </si>
+  <si>
+    <t>coke_oven_coal_consumption</t>
   </si>
 </sst>
 </file>
@@ -896,7 +899,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1097,8 +1100,8 @@
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>72</v>
+      <c r="B12" t="s">
+        <v>90</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>84</v>

</xml_diff>

<commit_message>
Change fugitive and other transformation to process emissions. Remove natural emission sectors.
</commit_message>
<xml_diff>
--- a/input/mappings/Master_Fuel_Sector_List.xlsx
+++ b/input/mappings/Master_Fuel_Sector_List.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13020" windowHeight="11880" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13020" windowHeight="11880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sectors" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="95">
   <si>
     <t>1A1a_Electricity-public</t>
   </si>
@@ -209,15 +209,6 @@
   </si>
   <si>
     <t>7A_Fossil-fuel-fires</t>
-  </si>
-  <si>
-    <t>11A_Volcanoes</t>
-  </si>
-  <si>
-    <t>11B_Forest-fires</t>
-  </si>
-  <si>
-    <t>11C_Other-natural</t>
   </si>
   <si>
     <t>sector</t>
@@ -320,7 +311,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -363,6 +354,22 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -381,9 +388,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -394,7 +405,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="6">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -727,21 +742,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -785,10 +804,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="D5" s="2"/>
     </row>
@@ -1085,10 +1104,10 @@
         <v>30</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="D30" s="2"/>
     </row>
@@ -1097,10 +1116,10 @@
         <v>31</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="D31" s="2"/>
     </row>
@@ -1109,10 +1128,10 @@
         <v>32</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="D32" s="2"/>
     </row>
@@ -1407,43 +1426,26 @@
       <c r="D56" s="2"/>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
       <c r="D57" s="2"/>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
       <c r="D58" s="2"/>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
       <c r="D59" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1456,7 +1458,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -1470,151 +1472,151 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15">
       <c r="A1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>72</v>
       </c>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" ht="15">
       <c r="A2" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>76</v>
       </c>
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" ht="15">
       <c r="A3" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>75</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>78</v>
       </c>
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" ht="15">
       <c r="A4" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" ht="15">
       <c r="A5" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>84</v>
       </c>
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" ht="15">
       <c r="A6" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>88</v>
       </c>
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" ht="15">
       <c r="A7" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>90</v>
       </c>
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" ht="15">
       <c r="A8" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="15">
       <c r="A9" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" ht="15">
       <c r="A10" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>97</v>
       </c>
       <c r="E10" s="5"/>
     </row>

</xml_diff>

<commit_message>
Revert to previous version. No changes.
</commit_message>
<xml_diff>
--- a/input/mappings/Master_Fuel_Sector_List.xlsx
+++ b/input/mappings/Master_Fuel_Sector_List.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13020" windowHeight="11880" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13020" windowHeight="11880" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sectors" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="98">
   <si>
     <t>1A1a_Electricity-public</t>
   </si>
@@ -209,6 +209,15 @@
   </si>
   <si>
     <t>7A_Fossil-fuel-fires</t>
+  </si>
+  <si>
+    <t>11A_Volcanoes</t>
+  </si>
+  <si>
+    <t>11B_Forest-fires</t>
+  </si>
+  <si>
+    <t>11C_Other-natural</t>
   </si>
   <si>
     <t>sector</t>
@@ -311,7 +320,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -354,22 +363,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -388,13 +381,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -405,11 +394,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -742,25 +727,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="29.1640625" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -804,10 +785,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="D5" s="2"/>
     </row>
@@ -1104,10 +1085,10 @@
         <v>30</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="D30" s="2"/>
     </row>
@@ -1116,10 +1097,10 @@
         <v>31</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="D31" s="2"/>
     </row>
@@ -1128,10 +1109,10 @@
         <v>32</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="D32" s="2"/>
     </row>
@@ -1426,26 +1407,43 @@
       <c r="D56" s="2"/>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
+      <c r="A57" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="D57" s="2"/>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
+      <c r="A58" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="D58" s="2"/>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
+      <c r="A59" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="D59" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1458,7 +1456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -1472,151 +1470,151 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15">
       <c r="A1" s="4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" ht="15">
       <c r="A2" s="5" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" ht="15">
       <c r="A3" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>71</v>
-      </c>
       <c r="C3" s="5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" ht="15">
       <c r="A4" s="5" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" ht="15">
       <c r="A5" s="5" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" ht="15">
       <c r="A6" s="5" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" ht="15">
       <c r="A7" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>83</v>
-      </c>
       <c r="C7" s="5" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" ht="15">
       <c r="A8" s="5" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="15">
       <c r="A9" s="5" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" ht="15">
       <c r="A10" s="5" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E10" s="5"/>
     </row>

</xml_diff>

<commit_message>
Change sectors 1A1bc and 1Bx to process emissions
</commit_message>
<xml_diff>
--- a/input/mappings/Master_Fuel_Sector_List.xlsx
+++ b/input/mappings/Master_Fuel_Sector_List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13020" windowHeight="11880" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16320" windowHeight="18220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sectors" sheetId="1" r:id="rId1"/>
@@ -320,7 +320,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -363,6 +363,22 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -381,9 +397,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -394,7 +412,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -727,11 +747,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="36.1640625" customWidth="1"/>
+    <col min="2" max="2" width="34" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
@@ -785,10 +809,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="D5" s="2"/>
     </row>
@@ -1085,10 +1109,10 @@
         <v>30</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="D30" s="2"/>
     </row>
@@ -1097,10 +1121,10 @@
         <v>31</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="D31" s="2"/>
     </row>
@@ -1109,10 +1133,10 @@
         <v>32</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="D32" s="2"/>
     </row>
@@ -1444,6 +1468,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1456,7 +1481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Remove older pulp and paper and smelting activity data
</commit_message>
<xml_diff>
--- a/input/mappings/Master_Fuel_Sector_List.xlsx
+++ b/input/mappings/Master_Fuel_Sector_List.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16320" windowHeight="18220" tabRatio="500"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="94">
   <si>
     <t>1A1a_Electricity-public</t>
   </si>
@@ -142,12 +142,6 @@
     <t>2C_Metal-production</t>
   </si>
   <si>
-    <t>Metal_S_Content</t>
-  </si>
-  <si>
-    <t>Default total S content of smelted metals</t>
-  </si>
-  <si>
     <t>2D_Degreasing-Cleaning</t>
   </si>
   <si>
@@ -161,12 +155,6 @@
   </si>
   <si>
     <t>2H_Pulp-and-paper-food-beverage-wood</t>
-  </si>
-  <si>
-    <t>Pulp_Paper_Production</t>
-  </si>
-  <si>
-    <t>tons</t>
   </si>
   <si>
     <t>2L_Other-process-emissions</t>
@@ -397,9 +385,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -412,9 +410,19 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="14">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -747,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:C5"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -759,13 +767,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1193,18 +1201,16 @@
         <v>39</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>41</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D37" s="1"/>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>34</v>
@@ -1216,7 +1222,7 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>34</v>
@@ -1228,7 +1234,7 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>34</v>
@@ -1240,7 +1246,7 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>34</v>
@@ -1252,19 +1258,19 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="D42" s="2"/>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>34</v>
@@ -1276,7 +1282,7 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>34</v>
@@ -1288,7 +1294,7 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>34</v>
@@ -1300,7 +1306,7 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>34</v>
@@ -1312,7 +1318,7 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>34</v>
@@ -1324,7 +1330,7 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>34</v>
@@ -1336,7 +1342,7 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>34</v>
@@ -1348,7 +1354,7 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>34</v>
@@ -1360,7 +1366,7 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>34</v>
@@ -1372,7 +1378,7 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>34</v>
@@ -1384,7 +1390,7 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>34</v>
@@ -1396,7 +1402,7 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>34</v>
@@ -1408,7 +1414,7 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>34</v>
@@ -1420,7 +1426,7 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>34</v>
@@ -1432,7 +1438,7 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>34</v>
@@ -1444,7 +1450,7 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>34</v>
@@ -1456,7 +1462,7 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>34</v>
@@ -1495,151 +1501,151 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15">
       <c r="A1" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" ht="15">
       <c r="A2" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" ht="15">
       <c r="A3" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>78</v>
       </c>
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" ht="15">
       <c r="A4" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" ht="15">
       <c r="A5" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" ht="15">
       <c r="A6" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" ht="15">
       <c r="A7" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>86</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>90</v>
       </c>
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" ht="15">
       <c r="A8" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="15">
       <c r="A9" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" ht="15">
       <c r="A10" s="5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E10" s="5"/>
     </row>

</xml_diff>

<commit_message>
Rearrange module D to calculate emissions from activity and ef. activity and ef dbs are same size for nc and comb emissions.
</commit_message>
<xml_diff>
--- a/input/mappings/Master_Fuel_Sector_List.xlsx
+++ b/input/mappings/Master_Fuel_Sector_List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16320" windowHeight="18220" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sectors" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="97">
   <si>
     <t>1A1a_Electricity-public</t>
   </si>
@@ -302,6 +302,15 @@
   </si>
   <si>
     <t>Process emissions- no fuel</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>comb</t>
+  </si>
+  <si>
+    <t>NC</t>
   </si>
 </sst>
 </file>
@@ -385,9 +394,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="14">
+  <cellStyleXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -410,19 +423,23 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="14">
+  <cellStyles count="18">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -755,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -775,6 +792,9 @@
       <c r="C1" s="3" t="s">
         <v>64</v>
       </c>
+      <c r="D1" s="3" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
@@ -786,7 +806,9 @@
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
@@ -798,7 +820,9 @@
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
@@ -810,7 +834,9 @@
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
@@ -822,7 +848,9 @@
       <c r="C5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
@@ -834,7 +862,9 @@
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
@@ -846,7 +876,9 @@
       <c r="C7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
@@ -858,7 +890,9 @@
       <c r="C8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
@@ -870,7 +904,9 @@
       <c r="C9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
@@ -882,7 +918,9 @@
       <c r="C10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
@@ -894,7 +932,9 @@
       <c r="C11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
@@ -906,7 +946,9 @@
       <c r="C12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
@@ -918,7 +960,9 @@
       <c r="C13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
@@ -930,7 +974,9 @@
       <c r="C14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
@@ -942,7 +988,9 @@
       <c r="C15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
@@ -954,7 +1002,9 @@
       <c r="C16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="2"/>
+      <c r="D16" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
@@ -966,7 +1016,9 @@
       <c r="C17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
@@ -978,7 +1030,9 @@
       <c r="C18" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="2"/>
+      <c r="D18" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
@@ -990,7 +1044,9 @@
       <c r="C19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="2"/>
+      <c r="D19" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
@@ -1002,7 +1058,9 @@
       <c r="C20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="2"/>
+      <c r="D20" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
@@ -1014,7 +1072,9 @@
       <c r="C21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="2"/>
+      <c r="D21" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
@@ -1026,7 +1086,9 @@
       <c r="C22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="2"/>
+      <c r="D22" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
@@ -1038,7 +1100,9 @@
       <c r="C23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="2"/>
+      <c r="D23" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
@@ -1050,7 +1114,9 @@
       <c r="C24" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="2"/>
+      <c r="D24" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
@@ -1062,7 +1128,9 @@
       <c r="C25" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D25" s="2"/>
+      <c r="D25" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
@@ -1074,7 +1142,9 @@
       <c r="C26" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D26" s="2"/>
+      <c r="D26" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
@@ -1086,7 +1156,9 @@
       <c r="C27" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="2"/>
+      <c r="D27" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
@@ -1098,7 +1170,9 @@
       <c r="C28" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D28" s="2"/>
+      <c r="D28" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1" t="s">
@@ -1110,7 +1184,9 @@
       <c r="C29" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="2"/>
+      <c r="D29" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
@@ -1122,7 +1198,9 @@
       <c r="C30" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D30" s="2"/>
+      <c r="D30" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
@@ -1134,7 +1212,9 @@
       <c r="C31" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="2"/>
+      <c r="D31" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="1" t="s">
@@ -1146,7 +1226,9 @@
       <c r="C32" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D32" s="2"/>
+      <c r="D32" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="1" t="s">
@@ -1158,7 +1240,9 @@
       <c r="C33" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D33" s="2"/>
+      <c r="D33" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
@@ -1170,7 +1254,9 @@
       <c r="C34" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D34" s="2"/>
+      <c r="D34" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="1" t="s">
@@ -1182,7 +1268,9 @@
       <c r="C35" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="2"/>
+      <c r="D35" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="1" t="s">
@@ -1194,7 +1282,9 @@
       <c r="C36" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D36" s="2"/>
+      <c r="D36" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="1" t="s">
@@ -1206,7 +1296,9 @@
       <c r="C37" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D37" s="1"/>
+      <c r="D37" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="1" t="s">
@@ -1218,7 +1310,9 @@
       <c r="C38" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D38" s="2"/>
+      <c r="D38" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="1" t="s">
@@ -1230,7 +1324,9 @@
       <c r="C39" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D39" s="2"/>
+      <c r="D39" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="1" t="s">
@@ -1242,7 +1338,9 @@
       <c r="C40" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D40" s="2"/>
+      <c r="D40" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="1" t="s">
@@ -1254,7 +1352,9 @@
       <c r="C41" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D41" s="2"/>
+      <c r="D41" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="1" t="s">
@@ -1266,7 +1366,9 @@
       <c r="C42" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D42" s="2"/>
+      <c r="D42" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="1" t="s">
@@ -1278,7 +1380,9 @@
       <c r="C43" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D43" s="2"/>
+      <c r="D43" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="1" t="s">
@@ -1290,7 +1394,9 @@
       <c r="C44" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D44" s="2"/>
+      <c r="D44" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="1" t="s">
@@ -1302,7 +1408,9 @@
       <c r="C45" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D45" s="2"/>
+      <c r="D45" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="1" t="s">
@@ -1314,7 +1422,9 @@
       <c r="C46" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D46" s="2"/>
+      <c r="D46" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="1" t="s">
@@ -1326,7 +1436,9 @@
       <c r="C47" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D47" s="2"/>
+      <c r="D47" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="1" t="s">
@@ -1338,7 +1450,9 @@
       <c r="C48" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D48" s="2"/>
+      <c r="D48" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="1" t="s">
@@ -1350,7 +1464,9 @@
       <c r="C49" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D49" s="2"/>
+      <c r="D49" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="1" t="s">
@@ -1362,7 +1478,9 @@
       <c r="C50" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D50" s="2"/>
+      <c r="D50" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="1" t="s">
@@ -1374,7 +1492,9 @@
       <c r="C51" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D51" s="2"/>
+      <c r="D51" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="1" t="s">
@@ -1386,7 +1506,9 @@
       <c r="C52" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D52" s="2"/>
+      <c r="D52" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="1" t="s">
@@ -1398,7 +1520,9 @@
       <c r="C53" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D53" s="2"/>
+      <c r="D53" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="1" t="s">
@@ -1410,7 +1534,9 @@
       <c r="C54" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D54" s="2"/>
+      <c r="D54" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="1" t="s">
@@ -1422,7 +1548,9 @@
       <c r="C55" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D55" s="2"/>
+      <c r="D55" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="1" t="s">
@@ -1434,7 +1562,9 @@
       <c r="C56" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D56" s="2"/>
+      <c r="D56" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="1" t="s">
@@ -1446,7 +1576,9 @@
       <c r="C57" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D57" s="2"/>
+      <c r="D57" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="1" t="s">
@@ -1458,7 +1590,9 @@
       <c r="C58" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D58" s="2"/>
+      <c r="D58" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="1" t="s">
@@ -1470,7 +1604,9 @@
       <c r="C59" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D59" s="2"/>
+      <c r="D59" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Change from GDP to population as the default process emission driver (since this is continuous throughout)
</commit_message>
<xml_diff>
--- a/input/mappings/Master_Fuel_Sector_List.xlsx
+++ b/input/mappings/Master_Fuel_Sector_List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14200" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25720" windowHeight="20260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sectors" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="96">
   <si>
     <t>1A1a_Electricity-public</t>
   </si>
@@ -124,12 +124,6 @@
     <t>2A1_Cement-production</t>
   </si>
   <si>
-    <t>GDP</t>
-  </si>
-  <si>
-    <t>B2005USD</t>
-  </si>
-  <si>
     <t>2A2_Lime-production</t>
   </si>
   <si>
@@ -311,6 +305,9 @@
   </si>
   <si>
     <t>NC</t>
+  </si>
+  <si>
+    <t>pop</t>
   </si>
 </sst>
 </file>
@@ -394,9 +391,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="18">
+  <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -423,7 +422,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="18">
+  <cellStyles count="20">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -432,6 +431,7 @@
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -440,6 +440,7 @@
     <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -772,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30:C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -784,16 +785,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -807,7 +808,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -821,7 +822,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -835,7 +836,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -843,13 +844,13 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>35</v>
+        <v>95</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1000</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -863,7 +864,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -877,7 +878,7 @@
         <v>2</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -891,7 +892,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -905,7 +906,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -919,7 +920,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -933,7 +934,7 @@
         <v>2</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -947,7 +948,7 @@
         <v>2</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -961,7 +962,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -975,7 +976,7 @@
         <v>2</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -989,7 +990,7 @@
         <v>2</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1003,7 +1004,7 @@
         <v>2</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1017,7 +1018,7 @@
         <v>2</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1031,7 +1032,7 @@
         <v>2</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1045,7 +1046,7 @@
         <v>2</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1059,7 +1060,7 @@
         <v>2</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1073,7 +1074,7 @@
         <v>2</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1087,7 +1088,7 @@
         <v>2</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1101,7 +1102,7 @@
         <v>2</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1115,7 +1116,7 @@
         <v>2</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1129,7 +1130,7 @@
         <v>2</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1143,7 +1144,7 @@
         <v>2</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1157,7 +1158,7 @@
         <v>2</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1171,7 +1172,7 @@
         <v>2</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1185,7 +1186,7 @@
         <v>2</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1193,13 +1194,13 @@
         <v>30</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>35</v>
+        <v>95</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1000</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1207,13 +1208,13 @@
         <v>31</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>35</v>
+        <v>95</v>
+      </c>
+      <c r="C31" s="1">
+        <v>1000</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1221,13 +1222,13 @@
         <v>32</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>35</v>
+        <v>95</v>
+      </c>
+      <c r="C32" s="1">
+        <v>1000</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1235,377 +1236,377 @@
         <v>33</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>35</v>
+        <v>95</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1000</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>35</v>
+        <v>95</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1000</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>35</v>
+        <v>95</v>
+      </c>
+      <c r="C35" s="1">
+        <v>1000</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>35</v>
+        <v>95</v>
+      </c>
+      <c r="C36" s="1">
+        <v>1000</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>35</v>
+        <v>95</v>
+      </c>
+      <c r="C37" s="1">
+        <v>1000</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>35</v>
+        <v>95</v>
+      </c>
+      <c r="C38" s="1">
+        <v>1000</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>35</v>
+        <v>95</v>
+      </c>
+      <c r="C39" s="1">
+        <v>1000</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>35</v>
+        <v>95</v>
+      </c>
+      <c r="C40" s="1">
+        <v>1000</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>35</v>
+        <v>95</v>
+      </c>
+      <c r="C41" s="1">
+        <v>1000</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>35</v>
+        <v>95</v>
+      </c>
+      <c r="C42" s="1">
+        <v>1000</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>35</v>
+        <v>95</v>
+      </c>
+      <c r="C43" s="1">
+        <v>1000</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>35</v>
+        <v>95</v>
+      </c>
+      <c r="C44" s="1">
+        <v>1000</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>35</v>
+        <v>95</v>
+      </c>
+      <c r="C45" s="1">
+        <v>1000</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>35</v>
+        <v>95</v>
+      </c>
+      <c r="C46" s="1">
+        <v>1000</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>35</v>
+        <v>95</v>
+      </c>
+      <c r="C47" s="1">
+        <v>1000</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>35</v>
+        <v>95</v>
+      </c>
+      <c r="C48" s="1">
+        <v>1000</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>35</v>
+        <v>95</v>
+      </c>
+      <c r="C49" s="1">
+        <v>1000</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>35</v>
+        <v>95</v>
+      </c>
+      <c r="C50" s="1">
+        <v>1000</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>35</v>
+        <v>95</v>
+      </c>
+      <c r="C51" s="1">
+        <v>1000</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>35</v>
+        <v>95</v>
+      </c>
+      <c r="C52" s="1">
+        <v>1000</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>35</v>
+        <v>95</v>
+      </c>
+      <c r="C53" s="1">
+        <v>1000</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>35</v>
+        <v>95</v>
+      </c>
+      <c r="C54" s="1">
+        <v>1000</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>35</v>
+        <v>95</v>
+      </c>
+      <c r="C55" s="1">
+        <v>1000</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>35</v>
+        <v>95</v>
+      </c>
+      <c r="C56" s="1">
+        <v>1000</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>35</v>
+        <v>95</v>
+      </c>
+      <c r="C57" s="1">
+        <v>1000</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>35</v>
+        <v>95</v>
+      </c>
+      <c r="C58" s="1">
+        <v>1000</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>35</v>
+        <v>95</v>
+      </c>
+      <c r="C59" s="1">
+        <v>1000</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1637,151 +1638,151 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15">
       <c r="A1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>68</v>
       </c>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" ht="15">
       <c r="A2" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>72</v>
       </c>
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" ht="15">
       <c r="A3" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" ht="15">
       <c r="A4" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" ht="15">
       <c r="A5" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>80</v>
       </c>
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" ht="15">
       <c r="A6" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="D6" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>84</v>
       </c>
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" ht="15">
       <c r="A7" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" ht="15">
       <c r="A8" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="15">
       <c r="A9" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>91</v>
       </c>
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" ht="15">
       <c r="A10" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E10" s="5"/>
     </row>

</xml_diff>

<commit_message>
Change drivers for fugitive emissions sectors
</commit_message>
<xml_diff>
--- a/input/mappings/Master_Fuel_Sector_List.xlsx
+++ b/input/mappings/Master_Fuel_Sector_List.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25720" windowHeight="20260" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sectors" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="98">
   <si>
     <t>1A1a_Electricity-public</t>
   </si>
@@ -308,6 +308,12 @@
   </si>
   <si>
     <t>pop</t>
+  </si>
+  <si>
+    <t>refinery-and-natural-gas</t>
+  </si>
+  <si>
+    <t>coal-dom-supply</t>
   </si>
 </sst>
 </file>
@@ -773,8 +779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:C59"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1193,11 +1199,11 @@
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C30" s="1">
-        <v>1000</v>
+      <c r="B30" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>94</v>
@@ -1207,11 +1213,11 @@
       <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C31" s="1">
-        <v>1000</v>
+      <c r="B31" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>94</v>
@@ -1221,11 +1227,11 @@
       <c r="A32" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C32" s="1">
-        <v>1000</v>
+      <c r="B32" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
Correct large problem with solid fuel fugitive emissions by going back to population as driver
</commit_message>
<xml_diff>
--- a/input/mappings/Master_Fuel_Sector_List.xlsx
+++ b/input/mappings/Master_Fuel_Sector_List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14640" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="14320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sectors" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="97">
   <si>
     <t>1A1a_Electricity-public</t>
   </si>
@@ -311,9 +311,6 @@
   </si>
   <si>
     <t>refinery-and-natural-gas</t>
-  </si>
-  <si>
-    <t>coal-dom-supply</t>
   </si>
 </sst>
 </file>
@@ -397,9 +394,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -428,7 +427,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="20">
+  <cellStyles count="22">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -438,6 +437,7 @@
     <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -447,6 +447,7 @@
     <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -1199,8 +1200,8 @@
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B30" t="s">
-        <v>97</v>
+      <c r="B30" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Fix error for solid fugitives sector, unit was inconsistent (so activity data was not applied)
</commit_message>
<xml_diff>
--- a/input/mappings/Master_Fuel_Sector_List.xlsx
+++ b/input/mappings/Master_Fuel_Sector_List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="14320" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sectors" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="97">
   <si>
     <t>1A1a_Electricity-public</t>
   </si>
@@ -394,9 +394,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -427,7 +429,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="22">
+  <cellStyles count="24">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -438,6 +440,7 @@
     <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -448,6 +451,7 @@
     <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -781,7 +785,7 @@
   <dimension ref="A1:D59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1203,8 +1207,8 @@
       <c r="B30" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>2</v>
+      <c r="C30" s="1">
+        <v>1000</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
Add pulp and paper consumption driver for waste burning
</commit_message>
<xml_diff>
--- a/input/mappings/Master_Fuel_Sector_List.xlsx
+++ b/input/mappings/Master_Fuel_Sector_List.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15500" yWindow="6420" windowWidth="25360" windowHeight="14640" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sectors" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="98">
   <si>
     <t>1A1a_Electricity-public</t>
   </si>
@@ -311,6 +311,9 @@
   </si>
   <si>
     <t>1A3dii_Domestic-navigation</t>
+  </si>
+  <si>
+    <t>pulp_paper_consumption</t>
   </si>
 </sst>
 </file>
@@ -784,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1513,10 +1516,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C52" s="1">
-        <v>1000</v>
+        <v>97</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>93</v>
@@ -1622,7 +1625,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1635,7 +1637,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -1799,7 +1801,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Added sector to 3 sector maps, reverted 4 mod-H files to pre-CEDS_Data to run Make
</commit_message>
<xml_diff>
--- a/input/mappings/Master_Fuel_Sector_List.xlsx
+++ b/input/mappings/Master_Fuel_Sector_List.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ben/mystuff/CEDS/input/mappings/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13940" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sectors" sheetId="1" r:id="rId1"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="99">
   <si>
     <t>1A1a_Electricity-public</t>
   </si>
@@ -314,6 +319,9 @@
   </si>
   <si>
     <t>pulp_paper_consumption</t>
+  </si>
+  <si>
+    <t>2L1_Oil-tanker-loading</t>
   </si>
 </sst>
 </file>
@@ -460,6 +468,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -785,19 +798,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="36.1640625" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>59</v>
       </c>
@@ -811,7 +824,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -825,7 +838,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -839,7 +852,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -853,7 +866,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -867,7 +880,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -881,7 +894,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -895,7 +908,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -909,7 +922,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -923,7 +936,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -937,7 +950,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -951,7 +964,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -965,7 +978,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -979,7 +992,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -993,7 +1006,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -1007,7 +1020,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1021,7 +1034,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -1035,7 +1048,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
@@ -1049,7 +1062,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -1063,7 +1076,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
@@ -1077,7 +1090,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
@@ -1091,7 +1104,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
@@ -1105,7 +1118,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
@@ -1119,7 +1132,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>96</v>
       </c>
@@ -1133,7 +1146,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -1147,7 +1160,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -1161,7 +1174,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -1175,7 +1188,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -1189,7 +1202,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -1203,7 +1216,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
@@ -1217,7 +1230,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
@@ -1231,7 +1244,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
@@ -1245,7 +1258,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
@@ -1259,7 +1272,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
@@ -1273,7 +1286,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
@@ -1287,7 +1300,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
@@ -1301,7 +1314,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
@@ -1315,7 +1328,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
@@ -1329,7 +1342,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
@@ -1343,7 +1356,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
@@ -1357,7 +1370,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
@@ -1371,7 +1384,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
@@ -1385,251 +1398,260 @@
         <v>93</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C43" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="1" t="s">
+      <c r="B44" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C44" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C44" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="1" t="s">
+      <c r="B45" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C45" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="1" t="s">
+      <c r="B46" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C46" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="1" t="s">
+      <c r="B47" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C47" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="1" t="s">
+      <c r="B48" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C48" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="1" t="s">
+      <c r="B49" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C49" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C49" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="1" t="s">
+      <c r="B50" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C50" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C50" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="1" t="s">
+      <c r="B51" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C51" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C51" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="1" t="s">
+      <c r="B52" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C52" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="1" t="s">
+      <c r="C53" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C53" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="1" t="s">
+      <c r="B54" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C54" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C54" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="1" t="s">
+      <c r="B55" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C55" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C55" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="1" t="s">
+      <c r="B56" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C56" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C56" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="1" t="s">
+      <c r="B57" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C57" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C57" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="1" t="s">
+      <c r="B58" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C58" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C58" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="1" t="s">
+      <c r="B59" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C59" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C59" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D59" s="2" t="s">
+      <c r="B60" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C60" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D60" s="2" t="s">
         <v>93</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1641,7 +1663,7 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="6"/>
     <col min="2" max="2" width="17" style="6" customWidth="1"/>
@@ -1649,7 +1671,7 @@
     <col min="4" max="16384" width="11" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>62</v>
       </c>
@@ -1664,7 +1686,7 @@
       </c>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:5" ht="15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>66</v>
       </c>
@@ -1679,7 +1701,7 @@
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:5" ht="15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>70</v>
       </c>
@@ -1694,7 +1716,7 @@
       </c>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:5" ht="15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>72</v>
       </c>
@@ -1709,7 +1731,7 @@
       </c>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" spans="1:5" ht="15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>74</v>
       </c>
@@ -1724,7 +1746,7 @@
       </c>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:5" ht="15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>78</v>
       </c>
@@ -1739,7 +1761,7 @@
       </c>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" ht="15">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>82</v>
       </c>
@@ -1754,7 +1776,7 @@
       </c>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5" ht="15">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>84</v>
       </c>
@@ -1769,7 +1791,7 @@
       </c>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" ht="15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>86</v>
       </c>
@@ -1784,7 +1806,7 @@
       </c>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" ht="15">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>89</v>
       </c>
@@ -1801,10 +1823,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed sector to 1A3di_Oil_Tanker_Loading to match Data_and_Assumptons summary
</commit_message>
<xml_diff>
--- a/input/mappings/Master_Fuel_Sector_List.xlsx
+++ b/input/mappings/Master_Fuel_Sector_List.xlsx
@@ -321,14 +321,14 @@
     <t>pulp_paper_consumption</t>
   </si>
   <si>
-    <t>2L1_Oil-tanker-loading</t>
+    <t>1A3di_Oil_Tanker_Loading</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -387,6 +387,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF24292E"/>
+      <name val="Helvetica"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -431,7 +436,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -439,6 +444,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="24">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -800,8 +806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1119,22 +1125,22 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>23</v>
+      <c r="A23" s="7" t="s">
+        <v>98</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>1</v>
+        <v>94</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>96</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>1</v>
@@ -1148,7 +1154,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>96</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>1</v>
@@ -1162,7 +1168,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>1</v>
@@ -1176,7 +1182,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>1</v>
@@ -1190,7 +1196,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>1</v>
@@ -1204,7 +1210,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>1</v>
@@ -1218,27 +1224,27 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C30" s="1">
-        <v>1000</v>
+        <v>1</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31" t="s">
-        <v>95</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>2</v>
+        <v>29</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" s="1">
+        <v>1000</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>93</v>
@@ -1246,7 +1252,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" t="s">
         <v>95</v>
@@ -1260,13 +1266,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C33" s="1">
-        <v>1000</v>
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>93</v>
@@ -1274,7 +1280,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>94</v>
@@ -1288,7 +1294,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>94</v>
@@ -1302,7 +1308,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>94</v>
@@ -1316,7 +1322,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>94</v>
@@ -1330,7 +1336,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>94</v>
@@ -1344,7 +1350,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>94</v>
@@ -1358,7 +1364,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>94</v>
@@ -1372,7 +1378,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>94</v>
@@ -1386,7 +1392,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>94</v>
@@ -1400,13 +1406,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>98</v>
+        <v>41</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>2</v>
+      <c r="C43" s="1">
+        <v>1000</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>93</v>

</xml_diff>

<commit_message>
Fix tracking other transformation through A6.1
</commit_message>
<xml_diff>
--- a/input/mappings/Master_Fuel_Sector_List.xlsx
+++ b/input/mappings/Master_Fuel_Sector_List.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -816,7 +816,7 @@
   <dimension ref="A1:D61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -900,7 +900,7 @@
         <v>99</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1</v>
+        <v>94</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Fixing some other transformation problems.
</commit_message>
<xml_diff>
--- a/input/mappings/Master_Fuel_Sector_List.xlsx
+++ b/input/mappings/Master_Fuel_Sector_List.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10523"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hoes919/Documents/CEDS/input/mappings/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA61578-570F-224A-9DC2-052936FEC2D7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +16,7 @@
     <sheet name="Sectors" sheetId="1" r:id="rId1"/>
     <sheet name="Fuels" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="103">
   <si>
     <t>1A1a_Electricity-public</t>
   </si>
@@ -328,6 +329,15 @@
   </si>
   <si>
     <t>1A1bc_Other-feedstocks</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>combustion</t>
+  </si>
+  <si>
+    <t>other</t>
   </si>
 </sst>
 </file>
@@ -813,869 +823,1053 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="36.1640625" customWidth="1"/>
-    <col min="2" max="2" width="34" customWidth="1"/>
+    <col min="2" max="2" width="23.5" customWidth="1"/>
+    <col min="3" max="3" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>98</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C32" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" t="s">
         <v>95</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D33" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" t="s">
         <v>95</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C35" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C36" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D36" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C37" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D37" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C38" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D38" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C39" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D39" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C40" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D40" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C41" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D41" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C42" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D42" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C43" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D43" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C44" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D44" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C45" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D45" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C46" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D46" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C47" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D47" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C48" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D48" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C49" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D49" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C50" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D50" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C51" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D51" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C52" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D52" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C53" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D53" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D54" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C55" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D55" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C56" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D56" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C57" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D57" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C58" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D58" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C59" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D59" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C60" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D60" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C61" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D61" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D61" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E61" s="2" t="s">
         <v>93</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update EDGAR processing and maps to include Indirect N2O sectors
- Modified "EDGAR_sector_comparison_map.csv" to include EDGAR sectors 4D3, 7B, and 7C ( no scaling sectors provided currently)
- Modified "Master_EDGAR_sector_mapping.csv" to include EDGAR sectors 4D3, 7B, and 7C ( no scaling sector provided currently)
- Modified "NC_EDGAR_sector_mapping.csv" to include EDGAR sectors 7B and 7C
- Modified "Edgar_scaling_mapping.xlsx" to include EDGAR sectors 4D3, 7B, and 7C (no scaling sector provided given that these EDGAR sectors are defaults in CEDS and don't need to be scaled)
- Modified "Master_Fuel_Sector_list.xlsx" to include new sector 7BC (indirect N2O from non-agg NH3 and NOx)
- Modified "Master_Sector_Level_map.csv" to include new sector 7BC (indirect N2O from non-agg NH3 and NOx)
</commit_message>
<xml_diff>
--- a/input/mappings/Master_Fuel_Sector_List.xlsx
+++ b/input/mappings/Master_Fuel_Sector_List.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26709"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20827"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ben/mystuff/CEDS/input/mappings/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orou913\Desktop\CEDS-Repositories\CEDS_N2O\CEDS\input\mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFAF8B57-835E-4DAE-B47D-E09B82A3DEEA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13940" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="13935" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sectors" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="100">
   <si>
     <t>1A1a_Electricity-public</t>
   </si>
@@ -322,13 +323,16 @@
   </si>
   <si>
     <t>1A3di_Oil_Tanker_Loading</t>
+  </si>
+  <si>
+    <t>7BC_Indirect-N2O-non-agricultural-N</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -387,11 +391,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF24292E"/>
-      <name val="Helvetica"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -436,7 +435,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -444,7 +443,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="24">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -470,13 +468,16 @@
     <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -803,20 +804,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.1640625" customWidth="1"/>
+    <col min="1" max="1" width="36.125" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>59</v>
       </c>
@@ -830,7 +831,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -844,7 +845,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -858,7 +859,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -872,7 +873,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -886,7 +887,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -900,7 +901,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -914,7 +915,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -928,7 +929,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -942,7 +943,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -956,7 +957,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -970,7 +971,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -984,7 +985,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -998,7 +999,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -1012,7 +1013,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -1026,7 +1027,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1040,7 +1041,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -1054,7 +1055,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
@@ -1068,7 +1069,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -1082,7 +1083,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
@@ -1096,7 +1097,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
@@ -1110,7 +1111,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
@@ -1124,8 +1125,8 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1138,7 +1139,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -1152,7 +1153,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>96</v>
       </c>
@@ -1166,7 +1167,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -1180,7 +1181,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -1194,7 +1195,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -1208,7 +1209,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -1222,7 +1223,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
@@ -1236,7 +1237,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
@@ -1250,7 +1251,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
@@ -1264,7 +1265,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
@@ -1278,7 +1279,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
@@ -1292,7 +1293,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
@@ -1306,7 +1307,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
@@ -1320,7 +1321,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
@@ -1334,7 +1335,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
@@ -1348,7 +1349,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
@@ -1362,7 +1363,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
@@ -1376,7 +1377,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
@@ -1390,7 +1391,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
@@ -1404,7 +1405,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
@@ -1418,7 +1419,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>42</v>
       </c>
@@ -1432,7 +1433,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
@@ -1446,7 +1447,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>44</v>
       </c>
@@ -1460,7 +1461,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>45</v>
       </c>
@@ -1474,7 +1475,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>46</v>
       </c>
@@ -1488,7 +1489,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
@@ -1502,7 +1503,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
@@ -1516,7 +1517,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>49</v>
       </c>
@@ -1530,7 +1531,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>50</v>
       </c>
@@ -1544,7 +1545,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>51</v>
       </c>
@@ -1558,7 +1559,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>52</v>
       </c>
@@ -1572,7 +1573,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>53</v>
       </c>
@@ -1586,7 +1587,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>54</v>
       </c>
@@ -1600,7 +1601,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>55</v>
       </c>
@@ -1614,45 +1615,59 @@
         <v>93</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C58" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C58" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
+      <c r="B59" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C59" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C59" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
+      <c r="B60" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C60" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C60" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D60" s="2" t="s">
+      <c r="B61" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C61" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D61" s="2" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1662,22 +1677,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" style="6"/>
     <col min="2" max="2" width="17" style="6" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="19.625" style="6" customWidth="1"/>
     <col min="4" max="16384" width="11" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>62</v>
       </c>
@@ -1692,7 +1707,7 @@
       </c>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>66</v>
       </c>
@@ -1707,7 +1722,7 @@
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>70</v>
       </c>
@@ -1722,7 +1737,7 @@
       </c>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>72</v>
       </c>
@@ -1737,7 +1752,7 @@
       </c>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>74</v>
       </c>
@@ -1752,7 +1767,7 @@
       </c>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>78</v>
       </c>
@@ -1767,7 +1782,7 @@
       </c>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>82</v>
       </c>
@@ -1782,7 +1797,7 @@
       </c>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>84</v>
       </c>
@@ -1797,7 +1812,7 @@
       </c>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>86</v>
       </c>
@@ -1812,7 +1827,7 @@
       </c>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>89</v>
       </c>

</xml_diff>

<commit_message>
Additonal fugitive petr. & NG sector work
- Begin adding N2O to mod. C GAINS emissions script
- Update Master Fuel Sector List to include new fugutive sectors
- Update GAINS country map to match master - Easter and Rest of Southern Africa isos remapped to Western Africa RCP region
- Add new fugitive sectors to GAINS fuel sector map
</commit_message>
<xml_diff>
--- a/input/mappings/Master_Fuel_Sector_List.xlsx
+++ b/input/mappings/Master_Fuel_Sector_List.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orou913\Desktop\CEDS-Repositories\CEDS_N2O\CEDS\input\mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFAF8B57-835E-4DAE-B47D-E09B82A3DEEA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF6B173-E56A-403C-9687-D20C5380442D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="13935" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6435" yWindow="780" windowWidth="19740" windowHeight="14475" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sectors" sheetId="1" r:id="rId1"/>
     <sheet name="Fuels" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="102">
   <si>
     <t>1A1a_Electricity-public</t>
   </si>
@@ -118,9 +118,6 @@
     <t>1B1_Fugitive-solid-fuels</t>
   </si>
   <si>
-    <t>1B2_Fugitive-petr-and-gas</t>
-  </si>
-  <si>
     <t>1B2d_Fugitive-other-energy</t>
   </si>
   <si>
@@ -326,6 +323,15 @@
   </si>
   <si>
     <t>7BC_Indirect-N2O-non-agricultural-N</t>
+  </si>
+  <si>
+    <t>1B2_Fugitive-petr</t>
+  </si>
+  <si>
+    <t>1B2b_Fugitive-NG-prod</t>
+  </si>
+  <si>
+    <t>1B2b_Fugitive-NG-distr</t>
   </si>
 </sst>
 </file>
@@ -344,6 +350,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -356,6 +363,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -369,11 +377,13 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -435,7 +445,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -443,6 +453,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="24">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -805,10 +816,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -819,16 +831,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -842,7 +854,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -856,7 +868,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -870,7 +882,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -878,13 +890,13 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C5" s="1">
         <v>1000</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -898,7 +910,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -912,7 +924,7 @@
         <v>2</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -926,7 +938,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -940,7 +952,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -954,7 +966,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -968,7 +980,7 @@
         <v>2</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -982,7 +994,7 @@
         <v>2</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -996,7 +1008,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1010,7 +1022,7 @@
         <v>2</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1024,7 +1036,7 @@
         <v>2</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1038,7 +1050,7 @@
         <v>2</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1052,7 +1064,7 @@
         <v>2</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1066,7 +1078,7 @@
         <v>2</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1080,7 +1092,7 @@
         <v>2</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1094,7 +1106,7 @@
         <v>2</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1108,7 +1120,7 @@
         <v>2</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1122,21 +1134,21 @@
         <v>2</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1150,12 +1162,12 @@
         <v>2</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>1</v>
@@ -1164,7 +1176,7 @@
         <v>2</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1178,7 +1190,7 @@
         <v>2</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1192,7 +1204,7 @@
         <v>2</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1206,7 +1218,7 @@
         <v>2</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1220,7 +1232,7 @@
         <v>2</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1234,7 +1246,7 @@
         <v>2</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1242,433 +1254,461 @@
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" t="s">
         <v>94</v>
       </c>
-      <c r="C31" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" t="s">
-        <v>95</v>
-      </c>
       <c r="C32" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>31</v>
+      <c r="A33" s="7" t="s">
+        <v>100</v>
       </c>
       <c r="B33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B34" s="1" t="s">
+      <c r="A34" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B34" t="s">
         <v>94</v>
       </c>
-      <c r="C34" s="1">
-        <v>1000</v>
+      <c r="C34" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35" t="s">
         <v>94</v>
       </c>
-      <c r="C35" s="1">
-        <v>1000</v>
+      <c r="C35" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C36" s="1">
         <v>1000</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C37" s="1">
         <v>1000</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C38" s="1">
         <v>1000</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C39" s="1">
         <v>1000</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C40" s="1">
         <v>1000</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C41" s="1">
         <v>1000</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C42" s="1">
         <v>1000</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C43" s="1">
         <v>1000</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C44" s="1">
         <v>1000</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C45" s="1">
         <v>1000</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C46" s="1">
         <v>1000</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C47" s="1">
         <v>1000</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C48" s="1">
         <v>1000</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C49" s="1">
         <v>1000</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C50" s="1">
         <v>1000</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C51" s="1">
         <v>1000</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C52" s="1">
         <v>1000</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>2</v>
+        <v>93</v>
+      </c>
+      <c r="C53" s="1">
+        <v>1000</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C54" s="1">
         <v>1000</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C55" s="1">
-        <v>1000</v>
+        <v>96</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C56" s="1">
         <v>1000</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C57" s="1">
         <v>1000</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>99</v>
+        <v>53</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C58" s="1">
         <v>1000</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C59" s="1">
         <v>1000</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>57</v>
+        <v>98</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C60" s="1">
         <v>1000</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C61" s="1">
         <v>1000</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C62" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C63" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1694,151 +1734,151 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>65</v>
       </c>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>71</v>
       </c>
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>73</v>
       </c>
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>77</v>
       </c>
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="D6" s="5" t="s">
         <v>80</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>81</v>
       </c>
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>85</v>
       </c>
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C9" s="5" t="s">
+      <c r="D9" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>88</v>
       </c>
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>90</v>
       </c>
       <c r="E10" s="5"/>
     </row>

</xml_diff>

<commit_message>
Update sector mapping files to include nitric and adipic acid sectors
</commit_message>
<xml_diff>
--- a/input/mappings/Master_Fuel_Sector_List.xlsx
+++ b/input/mappings/Master_Fuel_Sector_List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orou913\Desktop\CEDS-Repositories\CEDS_N2O_bring_in_master\CEDS\input\mappings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickorourke/Desktop/CEDS-dev/input/mappings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E58CD8-CD9A-4929-A3AE-0D206BC83540}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4D6C16-FB4C-1347-91D0-EFBAD3FF3726}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="3855" windowWidth="22185" windowHeight="10815" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2620" yWindow="1900" windowWidth="22180" windowHeight="10820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sectors" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="108">
   <si>
     <t>1A1a_Electricity-public</t>
   </si>
@@ -344,6 +344,12 @@
   </si>
   <si>
     <t>1A1bc_Other-feedstocks</t>
+  </si>
+  <si>
+    <t>2B2_Chemicals-Nitric-acid</t>
+  </si>
+  <si>
+    <t>2B3_Chemicals-Adipic-acid</t>
   </si>
 </sst>
 </file>
@@ -813,20 +819,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E64"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B59" sqref="B59"/>
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.125" customWidth="1"/>
+    <col min="1" max="1" width="36.1640625" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>58</v>
       </c>
@@ -843,7 +849,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -860,7 +866,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -877,7 +883,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -894,7 +900,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -911,7 +917,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>105</v>
       </c>
@@ -928,7 +934,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -945,7 +951,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -962,7 +968,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -979,7 +985,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -996,7 +1002,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1013,7 +1019,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1030,7 +1036,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1047,7 +1053,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1064,7 +1070,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1081,7 +1087,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1098,7 +1104,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1115,7 +1121,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1132,7 +1138,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1149,7 +1155,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1166,7 +1172,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1183,7 +1189,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1200,7 +1206,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1217,7 +1223,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>97</v>
       </c>
@@ -1234,7 +1240,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1251,7 +1257,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>95</v>
       </c>
@@ -1268,7 +1274,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -1285,7 +1291,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -1302,7 +1308,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -1319,7 +1325,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -1336,7 +1342,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -1353,7 +1359,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -1370,7 +1376,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>99</v>
       </c>
@@ -1387,7 +1393,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>100</v>
       </c>
@@ -1404,7 +1410,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>101</v>
       </c>
@@ -1421,7 +1427,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>30</v>
       </c>
@@ -1438,7 +1444,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>31</v>
       </c>
@@ -1455,7 +1461,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>32</v>
       </c>
@@ -1472,7 +1478,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>33</v>
       </c>
@@ -1489,7 +1495,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>34</v>
       </c>
@@ -1506,411 +1512,445 @@
         <v>92</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>106</v>
+      </c>
+      <c r="B41" t="s">
+        <v>88</v>
+      </c>
+      <c r="C41" t="s">
+        <v>93</v>
+      </c>
+      <c r="D41">
+        <v>1000</v>
+      </c>
+      <c r="E41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>107</v>
+      </c>
+      <c r="B42" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" t="s">
+        <v>93</v>
+      </c>
+      <c r="D42">
+        <v>1000</v>
+      </c>
+      <c r="E42" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>35</v>
       </c>
-      <c r="B41" t="s">
-        <v>88</v>
-      </c>
-      <c r="C41" t="s">
-        <v>93</v>
-      </c>
-      <c r="D41">
-        <v>1000</v>
-      </c>
-      <c r="E41" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="B43" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" t="s">
+        <v>93</v>
+      </c>
+      <c r="D43">
+        <v>1000</v>
+      </c>
+      <c r="E43" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>36</v>
       </c>
-      <c r="B42" t="s">
-        <v>88</v>
-      </c>
-      <c r="C42" t="s">
-        <v>93</v>
-      </c>
-      <c r="D42">
-        <v>1000</v>
-      </c>
-      <c r="E42" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="B44" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44" t="s">
+        <v>93</v>
+      </c>
+      <c r="D44">
+        <v>1000</v>
+      </c>
+      <c r="E44" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>37</v>
       </c>
-      <c r="B43" t="s">
-        <v>88</v>
-      </c>
-      <c r="C43" t="s">
-        <v>93</v>
-      </c>
-      <c r="D43">
-        <v>1000</v>
-      </c>
-      <c r="E43" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="B45" t="s">
+        <v>88</v>
+      </c>
+      <c r="C45" t="s">
+        <v>93</v>
+      </c>
+      <c r="D45">
+        <v>1000</v>
+      </c>
+      <c r="E45" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>38</v>
       </c>
-      <c r="B44" t="s">
-        <v>88</v>
-      </c>
-      <c r="C44" t="s">
-        <v>93</v>
-      </c>
-      <c r="D44">
-        <v>1000</v>
-      </c>
-      <c r="E44" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="B46" t="s">
+        <v>88</v>
+      </c>
+      <c r="C46" t="s">
+        <v>93</v>
+      </c>
+      <c r="D46">
+        <v>1000</v>
+      </c>
+      <c r="E46" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>39</v>
       </c>
-      <c r="B45" t="s">
-        <v>88</v>
-      </c>
-      <c r="C45" t="s">
-        <v>93</v>
-      </c>
-      <c r="D45">
-        <v>1000</v>
-      </c>
-      <c r="E45" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="B47" t="s">
+        <v>88</v>
+      </c>
+      <c r="C47" t="s">
+        <v>93</v>
+      </c>
+      <c r="D47">
+        <v>1000</v>
+      </c>
+      <c r="E47" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>40</v>
       </c>
-      <c r="B46" t="s">
-        <v>88</v>
-      </c>
-      <c r="C46" t="s">
-        <v>93</v>
-      </c>
-      <c r="D46">
-        <v>1000</v>
-      </c>
-      <c r="E46" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="B48" t="s">
+        <v>88</v>
+      </c>
+      <c r="C48" t="s">
+        <v>93</v>
+      </c>
+      <c r="D48">
+        <v>1000</v>
+      </c>
+      <c r="E48" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>41</v>
       </c>
-      <c r="B47" t="s">
-        <v>88</v>
-      </c>
-      <c r="C47" t="s">
-        <v>93</v>
-      </c>
-      <c r="D47">
-        <v>1000</v>
-      </c>
-      <c r="E47" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="B49" t="s">
+        <v>88</v>
+      </c>
+      <c r="C49" t="s">
+        <v>93</v>
+      </c>
+      <c r="D49">
+        <v>1000</v>
+      </c>
+      <c r="E49" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>42</v>
       </c>
-      <c r="B48" t="s">
-        <v>88</v>
-      </c>
-      <c r="C48" t="s">
-        <v>93</v>
-      </c>
-      <c r="D48">
-        <v>1000</v>
-      </c>
-      <c r="E48" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="B50" t="s">
+        <v>88</v>
+      </c>
+      <c r="C50" t="s">
+        <v>93</v>
+      </c>
+      <c r="D50">
+        <v>1000</v>
+      </c>
+      <c r="E50" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>43</v>
       </c>
-      <c r="B49" t="s">
-        <v>88</v>
-      </c>
-      <c r="C49" t="s">
-        <v>93</v>
-      </c>
-      <c r="D49">
-        <v>1000</v>
-      </c>
-      <c r="E49" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="B51" t="s">
+        <v>88</v>
+      </c>
+      <c r="C51" t="s">
+        <v>93</v>
+      </c>
+      <c r="D51">
+        <v>1000</v>
+      </c>
+      <c r="E51" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>44</v>
       </c>
-      <c r="B50" t="s">
-        <v>88</v>
-      </c>
-      <c r="C50" t="s">
-        <v>93</v>
-      </c>
-      <c r="D50">
-        <v>1000</v>
-      </c>
-      <c r="E50" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="B52" t="s">
+        <v>88</v>
+      </c>
+      <c r="C52" t="s">
+        <v>93</v>
+      </c>
+      <c r="D52">
+        <v>1000</v>
+      </c>
+      <c r="E52" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>45</v>
       </c>
-      <c r="B51" t="s">
-        <v>88</v>
-      </c>
-      <c r="C51" t="s">
-        <v>93</v>
-      </c>
-      <c r="D51">
-        <v>1000</v>
-      </c>
-      <c r="E51" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="B53" t="s">
+        <v>88</v>
+      </c>
+      <c r="C53" t="s">
+        <v>93</v>
+      </c>
+      <c r="D53">
+        <v>1000</v>
+      </c>
+      <c r="E53" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>46</v>
       </c>
-      <c r="B52" t="s">
-        <v>88</v>
-      </c>
-      <c r="C52" t="s">
-        <v>93</v>
-      </c>
-      <c r="D52">
-        <v>1000</v>
-      </c>
-      <c r="E52" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="B54" t="s">
+        <v>88</v>
+      </c>
+      <c r="C54" t="s">
+        <v>93</v>
+      </c>
+      <c r="D54">
+        <v>1000</v>
+      </c>
+      <c r="E54" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>47</v>
       </c>
-      <c r="B53" t="s">
-        <v>88</v>
-      </c>
-      <c r="C53" t="s">
-        <v>93</v>
-      </c>
-      <c r="D53">
-        <v>1000</v>
-      </c>
-      <c r="E53" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="B55" t="s">
+        <v>88</v>
+      </c>
+      <c r="C55" t="s">
+        <v>93</v>
+      </c>
+      <c r="D55">
+        <v>1000</v>
+      </c>
+      <c r="E55" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>48</v>
       </c>
-      <c r="B54" t="s">
-        <v>88</v>
-      </c>
-      <c r="C54" t="s">
-        <v>93</v>
-      </c>
-      <c r="D54">
-        <v>1000</v>
-      </c>
-      <c r="E54" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="B56" t="s">
+        <v>88</v>
+      </c>
+      <c r="C56" t="s">
+        <v>93</v>
+      </c>
+      <c r="D56">
+        <v>1000</v>
+      </c>
+      <c r="E56" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>49</v>
       </c>
-      <c r="B55" t="s">
-        <v>88</v>
-      </c>
-      <c r="C55" t="s">
-        <v>93</v>
-      </c>
-      <c r="D55">
-        <v>1000</v>
-      </c>
-      <c r="E55" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="B57" t="s">
+        <v>88</v>
+      </c>
+      <c r="C57" t="s">
+        <v>93</v>
+      </c>
+      <c r="D57">
+        <v>1000</v>
+      </c>
+      <c r="E57" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>50</v>
       </c>
-      <c r="B56" t="s">
-        <v>88</v>
-      </c>
-      <c r="C56" t="s">
+      <c r="B58" t="s">
+        <v>88</v>
+      </c>
+      <c r="C58" t="s">
         <v>96</v>
       </c>
-      <c r="D56" t="s">
-        <v>2</v>
-      </c>
-      <c r="E56" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="D58" t="s">
+        <v>2</v>
+      </c>
+      <c r="E58" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>51</v>
       </c>
-      <c r="B57" t="s">
-        <v>88</v>
-      </c>
-      <c r="C57" t="s">
-        <v>93</v>
-      </c>
-      <c r="D57">
-        <v>1000</v>
-      </c>
-      <c r="E57" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="B59" t="s">
+        <v>88</v>
+      </c>
+      <c r="C59" t="s">
+        <v>93</v>
+      </c>
+      <c r="D59">
+        <v>1000</v>
+      </c>
+      <c r="E59" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>52</v>
       </c>
-      <c r="B58" t="s">
-        <v>88</v>
-      </c>
-      <c r="C58" t="s">
-        <v>93</v>
-      </c>
-      <c r="D58">
-        <v>1000</v>
-      </c>
-      <c r="E58" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="B60" t="s">
+        <v>88</v>
+      </c>
+      <c r="C60" t="s">
+        <v>93</v>
+      </c>
+      <c r="D60">
+        <v>1000</v>
+      </c>
+      <c r="E60" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>53</v>
       </c>
-      <c r="B59" t="s">
-        <v>88</v>
-      </c>
-      <c r="C59" t="s">
-        <v>93</v>
-      </c>
-      <c r="D59">
-        <v>1000</v>
-      </c>
-      <c r="E59" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="B61" t="s">
+        <v>88</v>
+      </c>
+      <c r="C61" t="s">
+        <v>93</v>
+      </c>
+      <c r="D61">
+        <v>1000</v>
+      </c>
+      <c r="E61" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>54</v>
       </c>
-      <c r="B60" t="s">
-        <v>88</v>
-      </c>
-      <c r="C60" t="s">
-        <v>93</v>
-      </c>
-      <c r="D60">
-        <v>1000</v>
-      </c>
-      <c r="E60" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="B62" t="s">
+        <v>88</v>
+      </c>
+      <c r="C62" t="s">
+        <v>93</v>
+      </c>
+      <c r="D62">
+        <v>1000</v>
+      </c>
+      <c r="E62" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>98</v>
       </c>
-      <c r="B61" t="s">
-        <v>88</v>
-      </c>
-      <c r="C61" t="s">
-        <v>93</v>
-      </c>
-      <c r="D61">
-        <v>1000</v>
-      </c>
-      <c r="E61" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+      <c r="B63" t="s">
+        <v>88</v>
+      </c>
+      <c r="C63" t="s">
+        <v>93</v>
+      </c>
+      <c r="D63">
+        <v>1000</v>
+      </c>
+      <c r="E63" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>55</v>
       </c>
-      <c r="B62" t="s">
-        <v>88</v>
-      </c>
-      <c r="C62" t="s">
-        <v>93</v>
-      </c>
-      <c r="D62">
-        <v>1000</v>
-      </c>
-      <c r="E62" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="B64" t="s">
+        <v>88</v>
+      </c>
+      <c r="C64" t="s">
+        <v>93</v>
+      </c>
+      <c r="D64">
+        <v>1000</v>
+      </c>
+      <c r="E64" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>56</v>
       </c>
-      <c r="B63" t="s">
-        <v>88</v>
-      </c>
-      <c r="C63" t="s">
-        <v>93</v>
-      </c>
-      <c r="D63">
-        <v>1000</v>
-      </c>
-      <c r="E63" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="B65" t="s">
+        <v>88</v>
+      </c>
+      <c r="C65" t="s">
+        <v>93</v>
+      </c>
+      <c r="D65">
+        <v>1000</v>
+      </c>
+      <c r="E65" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>57</v>
       </c>
-      <c r="B64" t="s">
-        <v>88</v>
-      </c>
-      <c r="C64" t="s">
-        <v>93</v>
-      </c>
-      <c r="D64">
-        <v>1000</v>
-      </c>
-      <c r="E64" t="s">
+      <c r="B66" t="s">
+        <v>88</v>
+      </c>
+      <c r="C66" t="s">
+        <v>93</v>
+      </c>
+      <c r="D66">
+        <v>1000</v>
+      </c>
+      <c r="E66" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1925,18 +1965,18 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="3"/>
     <col min="2" max="2" width="17" style="3" customWidth="1"/>
-    <col min="3" max="3" width="19.625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" style="3" customWidth="1"/>
     <col min="4" max="16384" width="11" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>61</v>
       </c>
@@ -1951,7 +1991,7 @@
       </c>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>65</v>
       </c>
@@ -1966,7 +2006,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>69</v>
       </c>
@@ -1981,7 +2021,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>71</v>
       </c>
@@ -1996,7 +2036,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>73</v>
       </c>
@@ -2011,7 +2051,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>77</v>
       </c>
@@ -2026,7 +2066,7 @@
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>81</v>
       </c>
@@ -2041,7 +2081,7 @@
       </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>83</v>
       </c>
@@ -2056,7 +2096,7 @@
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>85</v>
       </c>
@@ -2071,7 +2111,7 @@
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
Updated crude oil production driver data to address discontinuities in original data
</commit_message>
<xml_diff>
--- a/input/mappings/Master_Fuel_Sector_List.xlsx
+++ b/input/mappings/Master_Fuel_Sector_List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickorourke/Desktop/CEDS-dev/input/mappings/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahsa361\OneDrive - PNNL\Documents\CEDS-dev2\input\mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4D6C16-FB4C-1347-91D0-EFBAD3FF3726}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{9A4D6C16-FB4C-1347-91D0-EFBAD3FF3726}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{40C6EE9D-1426-464E-85FA-A6314AFC2AE1}"/>
   <bookViews>
-    <workbookView xWindow="2620" yWindow="1900" windowWidth="22180" windowHeight="10820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34800" yWindow="2685" windowWidth="21600" windowHeight="11325" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sectors" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="109">
   <si>
     <t>1A1a_Electricity-public</t>
   </si>
@@ -350,6 +350,9 @@
   </si>
   <si>
     <t>2B3_Chemicals-Adipic-acid</t>
+  </si>
+  <si>
+    <t>fossil_fuel_production</t>
   </si>
 </sst>
 </file>
@@ -822,17 +825,18 @@
   <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A40" sqref="A40"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.1640625" customWidth="1"/>
+    <col min="1" max="1" width="36.19921875" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
+    <col min="3" max="3" width="22.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>58</v>
       </c>
@@ -849,7 +853,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -866,7 +870,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -883,7 +887,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -900,7 +904,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -917,7 +921,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>105</v>
       </c>
@@ -934,7 +938,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -951,7 +955,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -968,7 +972,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -985,7 +989,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1002,7 +1006,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1019,7 +1023,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1036,7 +1040,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1053,7 +1057,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1070,7 +1074,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1087,7 +1091,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1104,7 +1108,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1121,7 +1125,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1138,7 +1142,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1155,7 +1159,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1172,7 +1176,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1189,7 +1193,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1206,7 +1210,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1223,7 +1227,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>97</v>
       </c>
@@ -1240,7 +1244,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1257,7 +1261,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>95</v>
       </c>
@@ -1274,7 +1278,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -1291,7 +1295,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -1308,7 +1312,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -1325,7 +1329,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -1342,7 +1346,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -1359,7 +1363,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -1376,7 +1380,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>99</v>
       </c>
@@ -1384,7 +1388,7 @@
         <v>88</v>
       </c>
       <c r="C33" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="D33" t="s">
         <v>2</v>
@@ -1393,7 +1397,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>100</v>
       </c>
@@ -1410,7 +1414,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>101</v>
       </c>
@@ -1427,7 +1431,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>30</v>
       </c>
@@ -1444,7 +1448,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>31</v>
       </c>
@@ -1461,7 +1465,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>32</v>
       </c>
@@ -1478,7 +1482,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>33</v>
       </c>
@@ -1495,7 +1499,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>34</v>
       </c>
@@ -1512,7 +1516,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>106</v>
       </c>
@@ -1529,7 +1533,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>107</v>
       </c>
@@ -1546,7 +1550,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>35</v>
       </c>
@@ -1563,7 +1567,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>36</v>
       </c>
@@ -1580,7 +1584,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>37</v>
       </c>
@@ -1597,7 +1601,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>38</v>
       </c>
@@ -1614,7 +1618,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>39</v>
       </c>
@@ -1631,7 +1635,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>40</v>
       </c>
@@ -1648,7 +1652,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>41</v>
       </c>
@@ -1665,7 +1669,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>42</v>
       </c>
@@ -1682,7 +1686,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>43</v>
       </c>
@@ -1699,7 +1703,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>44</v>
       </c>
@@ -1716,7 +1720,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>45</v>
       </c>
@@ -1733,7 +1737,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>46</v>
       </c>
@@ -1750,7 +1754,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>47</v>
       </c>
@@ -1767,7 +1771,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>48</v>
       </c>
@@ -1784,7 +1788,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>49</v>
       </c>
@@ -1801,7 +1805,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>50</v>
       </c>
@@ -1818,7 +1822,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>51</v>
       </c>
@@ -1835,7 +1839,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>52</v>
       </c>
@@ -1852,7 +1856,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>53</v>
       </c>
@@ -1869,7 +1873,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>54</v>
       </c>
@@ -1886,7 +1890,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>98</v>
       </c>
@@ -1903,7 +1907,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>55</v>
       </c>
@@ -1920,7 +1924,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>56</v>
       </c>
@@ -1937,7 +1941,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>57</v>
       </c>
@@ -1968,15 +1972,15 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" style="3"/>
     <col min="2" max="2" width="17" style="3" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="19.69921875" style="3" customWidth="1"/>
     <col min="4" max="16384" width="11" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>61</v>
       </c>
@@ -1991,7 +1995,7 @@
       </c>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>65</v>
       </c>
@@ -2006,7 +2010,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>69</v>
       </c>
@@ -2021,7 +2025,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>71</v>
       </c>
@@ -2036,7 +2040,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>73</v>
       </c>
@@ -2051,7 +2055,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>77</v>
       </c>
@@ -2066,7 +2070,7 @@
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>81</v>
       </c>
@@ -2081,7 +2085,7 @@
       </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>83</v>
       </c>
@@ -2096,7 +2100,7 @@
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>85</v>
       </c>
@@ -2111,7 +2115,7 @@
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
Rename Hyde input date, delete unneeded years and IEA data Fix N2O year error with N2O 2B EDGAR merge Clarify crude oil production driver Extend diagnostics
</commit_message>
<xml_diff>
--- a/input/mappings/Master_Fuel_Sector_List.xlsx
+++ b/input/mappings/Master_Fuel_Sector_List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11213"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahsa361\OneDrive - PNNL\Documents\CEDS-dev2\input\mappings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Documents/Information &amp; Documents/CEDS_Project/CEDS/input/mappings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{9A4D6C16-FB4C-1347-91D0-EFBAD3FF3726}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{40C6EE9D-1426-464E-85FA-A6314AFC2AE1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4084280E-4680-684C-880D-BF6ACA16EF33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34800" yWindow="2685" windowWidth="21600" windowHeight="11325" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sectors" sheetId="1" r:id="rId1"/>
@@ -352,7 +352,7 @@
     <t>2B3_Chemicals-Adipic-acid</t>
   </si>
   <si>
-    <t>fossil_fuel_production</t>
+    <t>crude_oil_production</t>
   </si>
 </sst>
 </file>
@@ -825,18 +825,18 @@
   <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.19921875" customWidth="1"/>
+    <col min="1" max="1" width="36.1640625" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="3" max="3" width="22.8984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>58</v>
       </c>
@@ -853,7 +853,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -870,7 +870,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -887,7 +887,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -904,7 +904,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -921,7 +921,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>105</v>
       </c>
@@ -938,7 +938,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -955,7 +955,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -972,7 +972,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -989,7 +989,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1125,7 +1125,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1193,7 +1193,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1210,7 +1210,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>97</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>95</v>
       </c>
@@ -1278,7 +1278,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -1346,7 +1346,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -1380,7 +1380,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>99</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>100</v>
       </c>
@@ -1414,7 +1414,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>101</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>30</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>31</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>32</v>
       </c>
@@ -1482,7 +1482,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>33</v>
       </c>
@@ -1499,7 +1499,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>34</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>106</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>107</v>
       </c>
@@ -1550,7 +1550,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>35</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>36</v>
       </c>
@@ -1584,7 +1584,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>37</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>38</v>
       </c>
@@ -1618,7 +1618,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>39</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>40</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>41</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>42</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>43</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>44</v>
       </c>
@@ -1720,7 +1720,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>45</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>46</v>
       </c>
@@ -1754,7 +1754,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>47</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>48</v>
       </c>
@@ -1788,7 +1788,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>49</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>50</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>51</v>
       </c>
@@ -1839,7 +1839,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>52</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>53</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>54</v>
       </c>
@@ -1890,7 +1890,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>98</v>
       </c>
@@ -1907,7 +1907,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>55</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>56</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>57</v>
       </c>
@@ -1972,15 +1972,15 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="3"/>
     <col min="2" max="2" width="17" style="3" customWidth="1"/>
-    <col min="3" max="3" width="19.69921875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" style="3" customWidth="1"/>
     <col min="4" max="16384" width="11" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>61</v>
       </c>
@@ -1995,7 +1995,7 @@
       </c>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>65</v>
       </c>
@@ -2010,7 +2010,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>69</v>
       </c>
@@ -2025,7 +2025,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>71</v>
       </c>
@@ -2040,7 +2040,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>73</v>
       </c>
@@ -2055,7 +2055,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>77</v>
       </c>
@@ -2070,7 +2070,7 @@
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>81</v>
       </c>
@@ -2085,7 +2085,7 @@
       </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>83</v>
       </c>
@@ -2100,7 +2100,7 @@
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>85</v>
       </c>
@@ -2115,7 +2115,7 @@
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
Reset Fugitive petr sector driver to generic so that all countries have values.
</commit_message>
<xml_diff>
--- a/input/mappings/Master_Fuel_Sector_List.xlsx
+++ b/input/mappings/Master_Fuel_Sector_List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Documents/Information &amp; Documents/CEDS_Project/CEDS/input/mappings/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickorourke/Desktop/CEDS-dev/input/mappings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4084280E-4680-684C-880D-BF6ACA16EF33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4D6C16-FB4C-1347-91D0-EFBAD3FF3726}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2620" yWindow="1900" windowWidth="22180" windowHeight="10820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sectors" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="108">
   <si>
     <t>1A1a_Electricity-public</t>
   </si>
@@ -350,9 +350,6 @@
   </si>
   <si>
     <t>2B3_Chemicals-Adipic-acid</t>
-  </si>
-  <si>
-    <t>crude_oil_production</t>
   </si>
 </sst>
 </file>
@@ -825,15 +822,14 @@
   <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="36.1640625" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="3" max="3" width="22.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -1388,7 +1384,7 @@
         <v>88</v>
       </c>
       <c r="C33" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="D33" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Further oil production driver and extension updates (#296)
* Add back Hyde data, fix diagnostics/warnings, update extension methods.
* Update extension instructions
* Updated the extension data set for fugitive petroleum emissions based on a hybrid of oil production and CDIAC oil and liquid CO2 (#295)
* Updates to diagnostics and utility functions

Co-authored-by: Hamza Ahsan <hamza.ahsan@pnnl.gov>
Co-authored-by: Steve Smith <ssmith@pnnl.gov>
</commit_message>
<xml_diff>
--- a/input/mappings/Master_Fuel_Sector_List.xlsx
+++ b/input/mappings/Master_Fuel_Sector_List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11213"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickorourke/Desktop/CEDS-dev/input/mappings/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Documents/Information &amp; Documents/CEDS_Project/CEDS-clean/input/mappings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4D6C16-FB4C-1347-91D0-EFBAD3FF3726}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3055F7B1-EBE8-BE49-9AFE-886F9521DE59}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2620" yWindow="1900" windowWidth="22180" windowHeight="10820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6580" yWindow="460" windowWidth="22180" windowHeight="10820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sectors" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="107">
   <si>
     <t>1A1a_Electricity-public</t>
   </si>
@@ -308,9 +308,6 @@
   </si>
   <si>
     <t>pop</t>
-  </si>
-  <si>
-    <t>refinery-and-natural-gas</t>
   </si>
   <si>
     <t>1A3dii_Domestic-navigation</t>
@@ -822,14 +819,15 @@
   <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A40" sqref="A40"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C34" sqref="C34:E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="36.1640625" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -837,7 +835,7 @@
         <v>58</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>59</v>
@@ -854,7 +852,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -871,7 +869,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -888,7 +886,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
@@ -905,7 +903,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C5" t="s">
         <v>93</v>
@@ -919,10 +917,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C6" t="s">
         <v>93</v>
@@ -939,7 +937,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
@@ -956,7 +954,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
@@ -973,7 +971,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
@@ -990,7 +988,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
@@ -1007,7 +1005,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
@@ -1024,7 +1022,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C12" t="s">
         <v>1</v>
@@ -1041,7 +1039,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C13" t="s">
         <v>1</v>
@@ -1058,7 +1056,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C14" t="s">
         <v>1</v>
@@ -1075,7 +1073,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C15" t="s">
         <v>1</v>
@@ -1092,7 +1090,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C16" t="s">
         <v>1</v>
@@ -1109,7 +1107,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C17" t="s">
         <v>1</v>
@@ -1126,7 +1124,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C18" t="s">
         <v>1</v>
@@ -1143,7 +1141,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C19" t="s">
         <v>1</v>
@@ -1160,7 +1158,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C20" t="s">
         <v>1</v>
@@ -1177,7 +1175,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C21" t="s">
         <v>1</v>
@@ -1194,7 +1192,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C22" t="s">
         <v>1</v>
@@ -1211,7 +1209,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C23" t="s">
         <v>1</v>
@@ -1225,10 +1223,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C24" t="s">
         <v>93</v>
@@ -1245,7 +1243,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C25" t="s">
         <v>1</v>
@@ -1259,10 +1257,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C26" t="s">
         <v>1</v>
@@ -1279,7 +1277,7 @@
         <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C27" t="s">
         <v>1</v>
@@ -1296,7 +1294,7 @@
         <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C28" t="s">
         <v>1</v>
@@ -1313,7 +1311,7 @@
         <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C29" t="s">
         <v>1</v>
@@ -1330,7 +1328,7 @@
         <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C30" t="s">
         <v>1</v>
@@ -1347,7 +1345,7 @@
         <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C31" t="s">
         <v>1</v>
@@ -1378,16 +1376,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B33" t="s">
         <v>88</v>
       </c>
       <c r="C33" t="s">
-        <v>94</v>
-      </c>
-      <c r="D33" t="s">
-        <v>2</v>
+        <v>93</v>
+      </c>
+      <c r="D33">
+        <v>1000</v>
       </c>
       <c r="E33" t="s">
         <v>92</v>
@@ -1395,16 +1393,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B34" t="s">
         <v>88</v>
       </c>
       <c r="C34" t="s">
-        <v>94</v>
-      </c>
-      <c r="D34" t="s">
-        <v>2</v>
+        <v>93</v>
+      </c>
+      <c r="D34">
+        <v>1000</v>
       </c>
       <c r="E34" t="s">
         <v>92</v>
@@ -1412,16 +1410,16 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B35" t="s">
         <v>88</v>
       </c>
       <c r="C35" t="s">
-        <v>94</v>
-      </c>
-      <c r="D35" t="s">
-        <v>2</v>
+        <v>93</v>
+      </c>
+      <c r="D35">
+        <v>1000</v>
       </c>
       <c r="E35" t="s">
         <v>92</v>
@@ -1435,10 +1433,10 @@
         <v>88</v>
       </c>
       <c r="C36" t="s">
-        <v>94</v>
-      </c>
-      <c r="D36" t="s">
-        <v>2</v>
+        <v>93</v>
+      </c>
+      <c r="D36">
+        <v>1000</v>
       </c>
       <c r="E36" t="s">
         <v>92</v>
@@ -1514,7 +1512,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B41" t="s">
         <v>88</v>
@@ -1531,7 +1529,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B42" t="s">
         <v>88</v>
@@ -1809,7 +1807,7 @@
         <v>88</v>
       </c>
       <c r="C58" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D58" t="s">
         <v>2</v>
@@ -1888,7 +1886,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B63" t="s">
         <v>88</v>

</xml_diff>

<commit_message>
Added 2C_Aluminum-production sector. (Added driver .xlsx data, created driver data processing script, updated Master_Fuel_Sector_List and Master_Sector_Level_map, and activity_input_mapping file).
</commit_message>
<xml_diff>
--- a/input/mappings/Master_Fuel_Sector_List.xlsx
+++ b/input/mappings/Master_Fuel_Sector_List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Documents/Information &amp; Documents/CEDS_Project/CEDS-clean/input/mappings/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pnnl-my.sharepoint.com/personal/andrea_mott_pnnl_gov/Documents/Documents/CEDS-dev3/input/mappings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3055F7B1-EBE8-BE49-9AFE-886F9521DE59}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{3055F7B1-EBE8-BE49-9AFE-886F9521DE59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{4C9A309D-2ECE-49A2-8D8A-5F3E948653DD}"/>
   <bookViews>
-    <workbookView xWindow="6580" yWindow="460" windowWidth="22180" windowHeight="10820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sectors" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="109">
   <si>
     <t>1A1a_Electricity-public</t>
   </si>
@@ -347,6 +347,12 @@
   </si>
   <si>
     <t>2B3_Chemicals-Adipic-acid</t>
+  </si>
+  <si>
+    <t>aluminum_production</t>
+  </si>
+  <si>
+    <t>2C3_Aluminum-production</t>
   </si>
 </sst>
 </file>
@@ -816,21 +822,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C34" sqref="C34:E36"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="36.1640625" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>58</v>
       </c>
@@ -847,7 +853,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -864,7 +870,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -881,7 +887,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -898,7 +904,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -915,7 +921,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>104</v>
       </c>
@@ -932,7 +938,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -949,7 +955,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -966,7 +972,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -983,7 +989,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1000,7 +1006,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1017,7 +1023,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1034,7 +1040,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1051,7 +1057,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1068,7 +1074,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1085,7 +1091,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1102,7 +1108,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1119,7 +1125,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1136,7 +1142,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1153,7 +1159,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1170,7 +1176,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1187,7 +1193,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1204,7 +1210,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1221,7 +1227,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>96</v>
       </c>
@@ -1238,7 +1244,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1255,7 +1261,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>94</v>
       </c>
@@ -1272,7 +1278,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -1289,7 +1295,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -1306,7 +1312,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -1323,7 +1329,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -1340,7 +1346,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -1357,7 +1363,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -1374,7 +1380,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>98</v>
       </c>
@@ -1391,7 +1397,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>99</v>
       </c>
@@ -1408,7 +1414,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>100</v>
       </c>
@@ -1425,7 +1431,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>30</v>
       </c>
@@ -1442,7 +1448,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>31</v>
       </c>
@@ -1459,7 +1465,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>32</v>
       </c>
@@ -1476,7 +1482,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>33</v>
       </c>
@@ -1493,7 +1499,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>34</v>
       </c>
@@ -1510,7 +1516,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>105</v>
       </c>
@@ -1527,7 +1533,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>106</v>
       </c>
@@ -1544,7 +1550,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>35</v>
       </c>
@@ -1561,394 +1567,411 @@
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
+        <v>108</v>
+      </c>
+      <c r="B44" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44" t="s">
+        <v>107</v>
+      </c>
+      <c r="D44" t="s">
+        <v>2</v>
+      </c>
+      <c r="E44" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
         <v>36</v>
       </c>
-      <c r="B44" t="s">
-        <v>88</v>
-      </c>
-      <c r="C44" t="s">
-        <v>93</v>
-      </c>
-      <c r="D44">
-        <v>1000</v>
-      </c>
-      <c r="E44" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+      <c r="B45" t="s">
+        <v>88</v>
+      </c>
+      <c r="C45" t="s">
+        <v>93</v>
+      </c>
+      <c r="D45">
+        <v>1000</v>
+      </c>
+      <c r="E45" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
         <v>37</v>
       </c>
-      <c r="B45" t="s">
-        <v>88</v>
-      </c>
-      <c r="C45" t="s">
-        <v>93</v>
-      </c>
-      <c r="D45">
-        <v>1000</v>
-      </c>
-      <c r="E45" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+      <c r="B46" t="s">
+        <v>88</v>
+      </c>
+      <c r="C46" t="s">
+        <v>93</v>
+      </c>
+      <c r="D46">
+        <v>1000</v>
+      </c>
+      <c r="E46" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
         <v>38</v>
       </c>
-      <c r="B46" t="s">
-        <v>88</v>
-      </c>
-      <c r="C46" t="s">
-        <v>93</v>
-      </c>
-      <c r="D46">
-        <v>1000</v>
-      </c>
-      <c r="E46" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+      <c r="B47" t="s">
+        <v>88</v>
+      </c>
+      <c r="C47" t="s">
+        <v>93</v>
+      </c>
+      <c r="D47">
+        <v>1000</v>
+      </c>
+      <c r="E47" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>39</v>
       </c>
-      <c r="B47" t="s">
-        <v>88</v>
-      </c>
-      <c r="C47" t="s">
-        <v>93</v>
-      </c>
-      <c r="D47">
-        <v>1000</v>
-      </c>
-      <c r="E47" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+      <c r="B48" t="s">
+        <v>88</v>
+      </c>
+      <c r="C48" t="s">
+        <v>93</v>
+      </c>
+      <c r="D48">
+        <v>1000</v>
+      </c>
+      <c r="E48" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
         <v>40</v>
       </c>
-      <c r="B48" t="s">
-        <v>88</v>
-      </c>
-      <c r="C48" t="s">
-        <v>93</v>
-      </c>
-      <c r="D48">
-        <v>1000</v>
-      </c>
-      <c r="E48" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+      <c r="B49" t="s">
+        <v>88</v>
+      </c>
+      <c r="C49" t="s">
+        <v>93</v>
+      </c>
+      <c r="D49">
+        <v>1000</v>
+      </c>
+      <c r="E49" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
         <v>41</v>
       </c>
-      <c r="B49" t="s">
-        <v>88</v>
-      </c>
-      <c r="C49" t="s">
-        <v>93</v>
-      </c>
-      <c r="D49">
-        <v>1000</v>
-      </c>
-      <c r="E49" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+      <c r="B50" t="s">
+        <v>88</v>
+      </c>
+      <c r="C50" t="s">
+        <v>93</v>
+      </c>
+      <c r="D50">
+        <v>1000</v>
+      </c>
+      <c r="E50" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
         <v>42</v>
       </c>
-      <c r="B50" t="s">
-        <v>88</v>
-      </c>
-      <c r="C50" t="s">
-        <v>93</v>
-      </c>
-      <c r="D50">
-        <v>1000</v>
-      </c>
-      <c r="E50" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+      <c r="B51" t="s">
+        <v>88</v>
+      </c>
+      <c r="C51" t="s">
+        <v>93</v>
+      </c>
+      <c r="D51">
+        <v>1000</v>
+      </c>
+      <c r="E51" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
         <v>43</v>
       </c>
-      <c r="B51" t="s">
-        <v>88</v>
-      </c>
-      <c r="C51" t="s">
-        <v>93</v>
-      </c>
-      <c r="D51">
-        <v>1000</v>
-      </c>
-      <c r="E51" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+      <c r="B52" t="s">
+        <v>88</v>
+      </c>
+      <c r="C52" t="s">
+        <v>93</v>
+      </c>
+      <c r="D52">
+        <v>1000</v>
+      </c>
+      <c r="E52" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
         <v>44</v>
       </c>
-      <c r="B52" t="s">
-        <v>88</v>
-      </c>
-      <c r="C52" t="s">
-        <v>93</v>
-      </c>
-      <c r="D52">
-        <v>1000</v>
-      </c>
-      <c r="E52" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+      <c r="B53" t="s">
+        <v>88</v>
+      </c>
+      <c r="C53" t="s">
+        <v>93</v>
+      </c>
+      <c r="D53">
+        <v>1000</v>
+      </c>
+      <c r="E53" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
         <v>45</v>
       </c>
-      <c r="B53" t="s">
-        <v>88</v>
-      </c>
-      <c r="C53" t="s">
-        <v>93</v>
-      </c>
-      <c r="D53">
-        <v>1000</v>
-      </c>
-      <c r="E53" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+      <c r="B54" t="s">
+        <v>88</v>
+      </c>
+      <c r="C54" t="s">
+        <v>93</v>
+      </c>
+      <c r="D54">
+        <v>1000</v>
+      </c>
+      <c r="E54" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
         <v>46</v>
       </c>
-      <c r="B54" t="s">
-        <v>88</v>
-      </c>
-      <c r="C54" t="s">
-        <v>93</v>
-      </c>
-      <c r="D54">
-        <v>1000</v>
-      </c>
-      <c r="E54" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+      <c r="B55" t="s">
+        <v>88</v>
+      </c>
+      <c r="C55" t="s">
+        <v>93</v>
+      </c>
+      <c r="D55">
+        <v>1000</v>
+      </c>
+      <c r="E55" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
         <v>47</v>
       </c>
-      <c r="B55" t="s">
-        <v>88</v>
-      </c>
-      <c r="C55" t="s">
-        <v>93</v>
-      </c>
-      <c r="D55">
-        <v>1000</v>
-      </c>
-      <c r="E55" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+      <c r="B56" t="s">
+        <v>88</v>
+      </c>
+      <c r="C56" t="s">
+        <v>93</v>
+      </c>
+      <c r="D56">
+        <v>1000</v>
+      </c>
+      <c r="E56" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
         <v>48</v>
       </c>
-      <c r="B56" t="s">
-        <v>88</v>
-      </c>
-      <c r="C56" t="s">
-        <v>93</v>
-      </c>
-      <c r="D56">
-        <v>1000</v>
-      </c>
-      <c r="E56" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+      <c r="B57" t="s">
+        <v>88</v>
+      </c>
+      <c r="C57" t="s">
+        <v>93</v>
+      </c>
+      <c r="D57">
+        <v>1000</v>
+      </c>
+      <c r="E57" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
         <v>49</v>
       </c>
-      <c r="B57" t="s">
-        <v>88</v>
-      </c>
-      <c r="C57" t="s">
-        <v>93</v>
-      </c>
-      <c r="D57">
-        <v>1000</v>
-      </c>
-      <c r="E57" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+      <c r="B58" t="s">
+        <v>88</v>
+      </c>
+      <c r="C58" t="s">
+        <v>93</v>
+      </c>
+      <c r="D58">
+        <v>1000</v>
+      </c>
+      <c r="E58" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
         <v>50</v>
       </c>
-      <c r="B58" t="s">
-        <v>88</v>
-      </c>
-      <c r="C58" t="s">
+      <c r="B59" t="s">
+        <v>88</v>
+      </c>
+      <c r="C59" t="s">
         <v>95</v>
       </c>
-      <c r="D58" t="s">
-        <v>2</v>
-      </c>
-      <c r="E58" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+      <c r="D59" t="s">
+        <v>2</v>
+      </c>
+      <c r="E59" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
         <v>51</v>
       </c>
-      <c r="B59" t="s">
-        <v>88</v>
-      </c>
-      <c r="C59" t="s">
-        <v>93</v>
-      </c>
-      <c r="D59">
-        <v>1000</v>
-      </c>
-      <c r="E59" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+      <c r="B60" t="s">
+        <v>88</v>
+      </c>
+      <c r="C60" t="s">
+        <v>93</v>
+      </c>
+      <c r="D60">
+        <v>1000</v>
+      </c>
+      <c r="E60" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
         <v>52</v>
       </c>
-      <c r="B60" t="s">
-        <v>88</v>
-      </c>
-      <c r="C60" t="s">
-        <v>93</v>
-      </c>
-      <c r="D60">
-        <v>1000</v>
-      </c>
-      <c r="E60" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+      <c r="B61" t="s">
+        <v>88</v>
+      </c>
+      <c r="C61" t="s">
+        <v>93</v>
+      </c>
+      <c r="D61">
+        <v>1000</v>
+      </c>
+      <c r="E61" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
         <v>53</v>
       </c>
-      <c r="B61" t="s">
-        <v>88</v>
-      </c>
-      <c r="C61" t="s">
-        <v>93</v>
-      </c>
-      <c r="D61">
-        <v>1000</v>
-      </c>
-      <c r="E61" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+      <c r="B62" t="s">
+        <v>88</v>
+      </c>
+      <c r="C62" t="s">
+        <v>93</v>
+      </c>
+      <c r="D62">
+        <v>1000</v>
+      </c>
+      <c r="E62" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
         <v>54</v>
       </c>
-      <c r="B62" t="s">
-        <v>88</v>
-      </c>
-      <c r="C62" t="s">
-        <v>93</v>
-      </c>
-      <c r="D62">
-        <v>1000</v>
-      </c>
-      <c r="E62" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+      <c r="B63" t="s">
+        <v>88</v>
+      </c>
+      <c r="C63" t="s">
+        <v>93</v>
+      </c>
+      <c r="D63">
+        <v>1000</v>
+      </c>
+      <c r="E63" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
         <v>97</v>
       </c>
-      <c r="B63" t="s">
-        <v>88</v>
-      </c>
-      <c r="C63" t="s">
-        <v>93</v>
-      </c>
-      <c r="D63">
-        <v>1000</v>
-      </c>
-      <c r="E63" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
+      <c r="B64" t="s">
+        <v>88</v>
+      </c>
+      <c r="C64" t="s">
+        <v>93</v>
+      </c>
+      <c r="D64">
+        <v>1000</v>
+      </c>
+      <c r="E64" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
         <v>55</v>
       </c>
-      <c r="B64" t="s">
-        <v>88</v>
-      </c>
-      <c r="C64" t="s">
-        <v>93</v>
-      </c>
-      <c r="D64">
-        <v>1000</v>
-      </c>
-      <c r="E64" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+      <c r="B65" t="s">
+        <v>88</v>
+      </c>
+      <c r="C65" t="s">
+        <v>93</v>
+      </c>
+      <c r="D65">
+        <v>1000</v>
+      </c>
+      <c r="E65" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
         <v>56</v>
       </c>
-      <c r="B65" t="s">
-        <v>88</v>
-      </c>
-      <c r="C65" t="s">
-        <v>93</v>
-      </c>
-      <c r="D65">
-        <v>1000</v>
-      </c>
-      <c r="E65" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+      <c r="B66" t="s">
+        <v>88</v>
+      </c>
+      <c r="C66" t="s">
+        <v>93</v>
+      </c>
+      <c r="D66">
+        <v>1000</v>
+      </c>
+      <c r="E66" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
         <v>57</v>
       </c>
-      <c r="B66" t="s">
-        <v>88</v>
-      </c>
-      <c r="C66" t="s">
-        <v>93</v>
-      </c>
-      <c r="D66">
-        <v>1000</v>
-      </c>
-      <c r="E66" t="s">
+      <c r="B67" t="s">
+        <v>88</v>
+      </c>
+      <c r="C67" t="s">
+        <v>93</v>
+      </c>
+      <c r="D67">
+        <v>1000</v>
+      </c>
+      <c r="E67" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1966,7 +1989,7 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11" style="3"/>
     <col min="2" max="2" width="17" style="3" customWidth="1"/>
@@ -1974,7 +1997,7 @@
     <col min="4" max="16384" width="11" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>61</v>
       </c>
@@ -1989,7 +2012,7 @@
       </c>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>65</v>
       </c>
@@ -2004,7 +2027,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>69</v>
       </c>
@@ -2019,7 +2042,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>71</v>
       </c>
@@ -2034,7 +2057,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>73</v>
       </c>
@@ -2049,7 +2072,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>77</v>
       </c>
@@ -2064,7 +2087,7 @@
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>81</v>
       </c>
@@ -2079,7 +2102,7 @@
       </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>83</v>
       </c>
@@ -2094,7 +2117,7 @@
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>85</v>
       </c>
@@ -2109,7 +2132,7 @@
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
Add 2C1_Iron-steel-alloy-prod and 2C4_Non-Ferrous-other-metals to master fuel secotr list and sector level map.
</commit_message>
<xml_diff>
--- a/input/mappings/Master_Fuel_Sector_List.xlsx
+++ b/input/mappings/Master_Fuel_Sector_List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pnnl-my.sharepoint.com/personal/andrea_mott_pnnl_gov/Documents/Documents/CEDS-dev3/input/mappings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{3055F7B1-EBE8-BE49-9AFE-886F9521DE59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{4C9A309D-2ECE-49A2-8D8A-5F3E948653DD}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{3055F7B1-EBE8-BE49-9AFE-886F9521DE59}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{398DA30A-801C-42AD-B1E1-E85D14553852}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sectors" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="112">
   <si>
     <t>1A1a_Electricity-public</t>
   </si>
@@ -353,6 +353,15 @@
   </si>
   <si>
     <t>2C3_Aluminum-production</t>
+  </si>
+  <si>
+    <t>pig_iron</t>
+  </si>
+  <si>
+    <t>2C1_Iron-steel-alloy-prod</t>
+  </si>
+  <si>
+    <t>2C4_Non-Ferrous-other-metals</t>
   </si>
 </sst>
 </file>
@@ -822,11 +831,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D45" sqref="D45"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1586,16 +1595,16 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>36</v>
+        <v>110</v>
       </c>
       <c r="B45" t="s">
         <v>88</v>
       </c>
       <c r="C45" t="s">
-        <v>93</v>
-      </c>
-      <c r="D45">
-        <v>1000</v>
+        <v>109</v>
+      </c>
+      <c r="D45" t="s">
+        <v>2</v>
       </c>
       <c r="E45" t="s">
         <v>92</v>
@@ -1603,7 +1612,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>37</v>
+        <v>111</v>
       </c>
       <c r="B46" t="s">
         <v>88</v>
@@ -1620,7 +1629,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B47" t="s">
         <v>88</v>
@@ -1637,7 +1646,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B48" t="s">
         <v>88</v>
@@ -1654,7 +1663,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B49" t="s">
         <v>88</v>
@@ -1671,7 +1680,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B50" t="s">
         <v>88</v>
@@ -1688,7 +1697,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B51" t="s">
         <v>88</v>
@@ -1705,7 +1714,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B52" t="s">
         <v>88</v>
@@ -1722,7 +1731,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B53" t="s">
         <v>88</v>
@@ -1739,7 +1748,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B54" t="s">
         <v>88</v>
@@ -1756,7 +1765,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B55" t="s">
         <v>88</v>
@@ -1773,7 +1782,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B56" t="s">
         <v>88</v>
@@ -1790,7 +1799,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B57" t="s">
         <v>88</v>
@@ -1807,7 +1816,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B58" t="s">
         <v>88</v>
@@ -1824,16 +1833,16 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B59" t="s">
         <v>88</v>
       </c>
       <c r="C59" t="s">
-        <v>95</v>
-      </c>
-      <c r="D59" t="s">
-        <v>2</v>
+        <v>93</v>
+      </c>
+      <c r="D59">
+        <v>1000</v>
       </c>
       <c r="E59" t="s">
         <v>92</v>
@@ -1841,7 +1850,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B60" t="s">
         <v>88</v>
@@ -1858,16 +1867,16 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B61" t="s">
         <v>88</v>
       </c>
       <c r="C61" t="s">
-        <v>93</v>
-      </c>
-      <c r="D61">
-        <v>1000</v>
+        <v>95</v>
+      </c>
+      <c r="D61" t="s">
+        <v>2</v>
       </c>
       <c r="E61" t="s">
         <v>92</v>
@@ -1875,7 +1884,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B62" t="s">
         <v>88</v>
@@ -1892,7 +1901,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B63" t="s">
         <v>88</v>
@@ -1909,7 +1918,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>97</v>
+        <v>53</v>
       </c>
       <c r="B64" t="s">
         <v>88</v>
@@ -1926,7 +1935,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B65" t="s">
         <v>88</v>
@@ -1943,7 +1952,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>56</v>
+        <v>97</v>
       </c>
       <c r="B66" t="s">
         <v>88</v>
@@ -1960,18 +1969,52 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
+        <v>55</v>
+      </c>
+      <c r="B67" t="s">
+        <v>88</v>
+      </c>
+      <c r="C67" t="s">
+        <v>93</v>
+      </c>
+      <c r="D67">
+        <v>1000</v>
+      </c>
+      <c r="E67" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>56</v>
+      </c>
+      <c r="B68" t="s">
+        <v>88</v>
+      </c>
+      <c r="C68" t="s">
+        <v>93</v>
+      </c>
+      <c r="D68">
+        <v>1000</v>
+      </c>
+      <c r="E68" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
         <v>57</v>
       </c>
-      <c r="B67" t="s">
-        <v>88</v>
-      </c>
-      <c r="C67" t="s">
-        <v>93</v>
-      </c>
-      <c r="D67">
-        <v>1000</v>
-      </c>
-      <c r="E67" t="s">
+      <c r="B69" t="s">
+        <v>88</v>
+      </c>
+      <c r="C69" t="s">
+        <v>93</v>
+      </c>
+      <c r="D69">
+        <v>1000</v>
+      </c>
+      <c r="E69" t="s">
         <v>92</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove the 2C_Metal-production sector. Remove 2C_Metal-production from EDGAR non-combustion emissions scripts (C1.2.add_NC_emissions_EDGAR.R and C2.1.base_NC_EF.R). Remove sector from Master_Sector_Level_map.csv, and historical extension files (activity and EF).
</commit_message>
<xml_diff>
--- a/input/mappings/Master_Fuel_Sector_List.xlsx
+++ b/input/mappings/Master_Fuel_Sector_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pnnl-my.sharepoint.com/personal/andrea_mott_pnnl_gov/Documents/Documents/CEDS-dev3/input/mappings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{3055F7B1-EBE8-BE49-9AFE-886F9521DE59}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3F971D05-C525-4C4B-8B0B-93CF8EC456B1}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{3055F7B1-EBE8-BE49-9AFE-886F9521DE59}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{EB165BCE-1E81-4177-A577-29C1DD834E65}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="3430" windowWidth="9600" windowHeight="4910" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sectors" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="111">
   <si>
     <t>1A1a_Electricity-public</t>
   </si>
@@ -131,9 +131,6 @@
   </si>
   <si>
     <t>2B_Chemical-industry</t>
-  </si>
-  <si>
-    <t>2C_Metal-production</t>
   </si>
   <si>
     <t>2D_Degreasing-Cleaning</t>
@@ -831,43 +828,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="79" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
+      <selection pane="bottomLeft" activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.1640625" customWidth="1"/>
+    <col min="1" max="1" width="36.125" customWidth="1"/>
     <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>60</v>
-      </c>
       <c r="E1" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -876,15 +873,15 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -893,15 +890,15 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
@@ -910,49 +907,49 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5">
+        <v>1000</v>
+      </c>
+      <c r="E5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>103</v>
       </c>
-      <c r="C5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D5">
-        <v>1000</v>
-      </c>
-      <c r="E5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>104</v>
-      </c>
       <c r="B6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D6" t="s">
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
@@ -961,15 +958,15 @@
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
@@ -978,15 +975,15 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
@@ -995,15 +992,15 @@
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
@@ -1012,15 +1009,15 @@
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
@@ -1029,15 +1026,15 @@
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C12" t="s">
         <v>1</v>
@@ -1046,15 +1043,15 @@
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C13" t="s">
         <v>1</v>
@@ -1063,15 +1060,15 @@
         <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C14" t="s">
         <v>1</v>
@@ -1080,15 +1077,15 @@
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C15" t="s">
         <v>1</v>
@@ -1097,15 +1094,15 @@
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C16" t="s">
         <v>1</v>
@@ -1114,15 +1111,15 @@
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C17" t="s">
         <v>1</v>
@@ -1131,15 +1128,15 @@
         <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C18" t="s">
         <v>1</v>
@@ -1148,15 +1145,15 @@
         <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C19" t="s">
         <v>1</v>
@@ -1165,15 +1162,15 @@
         <v>2</v>
       </c>
       <c r="E19" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C20" t="s">
         <v>1</v>
@@ -1182,15 +1179,15 @@
         <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C21" t="s">
         <v>1</v>
@@ -1199,15 +1196,15 @@
         <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C22" t="s">
         <v>1</v>
@@ -1216,15 +1213,15 @@
         <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C23" t="s">
         <v>1</v>
@@ -1233,32 +1230,32 @@
         <v>2</v>
       </c>
       <c r="E23" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D24" t="s">
         <v>2</v>
       </c>
       <c r="E24" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C25" t="s">
         <v>1</v>
@@ -1267,15 +1264,15 @@
         <v>2</v>
       </c>
       <c r="E25" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C26" t="s">
         <v>1</v>
@@ -1284,15 +1281,15 @@
         <v>2</v>
       </c>
       <c r="E26" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C27" t="s">
         <v>1</v>
@@ -1301,15 +1298,15 @@
         <v>2</v>
       </c>
       <c r="E27" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C28" t="s">
         <v>1</v>
@@ -1318,15 +1315,15 @@
         <v>2</v>
       </c>
       <c r="E28" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C29" t="s">
         <v>1</v>
@@ -1335,15 +1332,15 @@
         <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C30" t="s">
         <v>1</v>
@@ -1352,15 +1349,15 @@
         <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C31" t="s">
         <v>1</v>
@@ -1369,653 +1366,636 @@
         <v>2</v>
       </c>
       <c r="E31" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D32">
         <v>1000</v>
       </c>
       <c r="E32" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>97</v>
+      </c>
+      <c r="B33" t="s">
+        <v>87</v>
+      </c>
+      <c r="C33" t="s">
+        <v>92</v>
+      </c>
+      <c r="D33">
+        <v>1000</v>
+      </c>
+      <c r="E33" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>98</v>
       </c>
-      <c r="B33" t="s">
-        <v>88</v>
-      </c>
-      <c r="C33" t="s">
-        <v>93</v>
-      </c>
-      <c r="D33">
-        <v>1000</v>
-      </c>
-      <c r="E33" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+      <c r="B34" t="s">
+        <v>87</v>
+      </c>
+      <c r="C34" t="s">
+        <v>92</v>
+      </c>
+      <c r="D34">
+        <v>1000</v>
+      </c>
+      <c r="E34" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>99</v>
       </c>
-      <c r="B34" t="s">
-        <v>88</v>
-      </c>
-      <c r="C34" t="s">
-        <v>93</v>
-      </c>
-      <c r="D34">
-        <v>1000</v>
-      </c>
-      <c r="E34" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>100</v>
-      </c>
       <c r="B35" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C35" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D35">
         <v>1000</v>
       </c>
       <c r="E35" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>30</v>
       </c>
       <c r="B36" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C36" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D36">
         <v>1000</v>
       </c>
       <c r="E36" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>31</v>
       </c>
       <c r="B37" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C37" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D37">
         <v>1000</v>
       </c>
       <c r="E37" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>32</v>
       </c>
       <c r="B38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D38">
         <v>1000</v>
       </c>
       <c r="E38" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>33</v>
       </c>
       <c r="B39" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C39" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D39">
         <v>1000</v>
       </c>
       <c r="E39" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>34</v>
       </c>
       <c r="B40" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C40" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D40">
         <v>1000</v>
       </c>
       <c r="E40" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>104</v>
+      </c>
+      <c r="B41" t="s">
+        <v>87</v>
+      </c>
+      <c r="C41" t="s">
+        <v>92</v>
+      </c>
+      <c r="D41">
+        <v>1000</v>
+      </c>
+      <c r="E41" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>105</v>
       </c>
-      <c r="B41" t="s">
-        <v>88</v>
-      </c>
-      <c r="C41" t="s">
-        <v>93</v>
-      </c>
-      <c r="D41">
-        <v>1000</v>
-      </c>
-      <c r="E41" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+      <c r="B42" t="s">
+        <v>87</v>
+      </c>
+      <c r="C42" t="s">
+        <v>92</v>
+      </c>
+      <c r="D42">
+        <v>1000</v>
+      </c>
+      <c r="E42" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>107</v>
+      </c>
+      <c r="B43" t="s">
+        <v>87</v>
+      </c>
+      <c r="C43" t="s">
         <v>106</v>
       </c>
-      <c r="B42" t="s">
-        <v>88</v>
-      </c>
-      <c r="C42" t="s">
-        <v>93</v>
-      </c>
-      <c r="D42">
-        <v>1000</v>
-      </c>
-      <c r="E42" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B43" t="s">
-        <v>88</v>
-      </c>
-      <c r="C43" t="s">
-        <v>93</v>
-      </c>
-      <c r="D43">
-        <v>1000</v>
+      <c r="D43" t="s">
+        <v>2</v>
       </c>
       <c r="E43" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>109</v>
+      </c>
+      <c r="B44" t="s">
+        <v>87</v>
+      </c>
+      <c r="C44" t="s">
         <v>108</v>
       </c>
-      <c r="B44" t="s">
-        <v>88</v>
-      </c>
-      <c r="C44" t="s">
-        <v>107</v>
-      </c>
       <c r="D44" t="s">
         <v>2</v>
       </c>
       <c r="E44" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>110</v>
       </c>
       <c r="B45" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C45" t="s">
-        <v>109</v>
-      </c>
-      <c r="D45" t="s">
-        <v>2</v>
+        <v>92</v>
+      </c>
+      <c r="D45">
+        <v>1000</v>
       </c>
       <c r="E45" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>111</v>
+        <v>35</v>
       </c>
       <c r="B46" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D46">
         <v>1000</v>
       </c>
       <c r="E46" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>36</v>
       </c>
       <c r="B47" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C47" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D47">
         <v>1000</v>
       </c>
       <c r="E47" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>37</v>
       </c>
       <c r="B48" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C48" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D48">
         <v>1000</v>
       </c>
       <c r="E48" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>38</v>
       </c>
       <c r="B49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C49" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D49">
         <v>1000</v>
       </c>
       <c r="E49" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>39</v>
       </c>
       <c r="B50" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C50" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D50">
         <v>1000</v>
       </c>
       <c r="E50" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>40</v>
       </c>
       <c r="B51" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C51" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D51">
         <v>1000</v>
       </c>
       <c r="E51" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>41</v>
       </c>
       <c r="B52" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C52" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D52">
         <v>1000</v>
       </c>
       <c r="E52" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>42</v>
       </c>
       <c r="B53" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C53" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D53">
         <v>1000</v>
       </c>
       <c r="E53" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>43</v>
       </c>
       <c r="B54" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C54" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D54">
         <v>1000</v>
       </c>
       <c r="E54" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>44</v>
       </c>
       <c r="B55" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C55" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D55">
         <v>1000</v>
       </c>
       <c r="E55" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>45</v>
       </c>
       <c r="B56" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D56">
         <v>1000</v>
       </c>
       <c r="E56" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>46</v>
       </c>
       <c r="B57" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C57" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D57">
         <v>1000</v>
       </c>
       <c r="E57" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>47</v>
       </c>
       <c r="B58" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C58" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D58">
         <v>1000</v>
       </c>
       <c r="E58" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>48</v>
       </c>
       <c r="B59" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C59" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D59">
         <v>1000</v>
       </c>
       <c r="E59" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>49</v>
       </c>
       <c r="B60" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C60" t="s">
-        <v>93</v>
-      </c>
-      <c r="D60">
-        <v>1000</v>
+        <v>94</v>
+      </c>
+      <c r="D60" t="s">
+        <v>2</v>
       </c>
       <c r="E60" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>50</v>
       </c>
       <c r="B61" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C61" t="s">
-        <v>95</v>
-      </c>
-      <c r="D61" t="s">
-        <v>2</v>
+        <v>92</v>
+      </c>
+      <c r="D61">
+        <v>1000</v>
       </c>
       <c r="E61" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>51</v>
       </c>
       <c r="B62" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C62" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D62">
         <v>1000</v>
       </c>
       <c r="E62" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>52</v>
       </c>
       <c r="B63" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C63" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D63">
         <v>1000</v>
       </c>
       <c r="E63" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>53</v>
       </c>
       <c r="B64" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C64" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D64">
         <v>1000</v>
       </c>
       <c r="E64" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>96</v>
+      </c>
+      <c r="B65" t="s">
+        <v>87</v>
+      </c>
+      <c r="C65" t="s">
+        <v>92</v>
+      </c>
+      <c r="D65">
+        <v>1000</v>
+      </c>
+      <c r="E65" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>54</v>
       </c>
-      <c r="B65" t="s">
-        <v>88</v>
-      </c>
-      <c r="C65" t="s">
-        <v>93</v>
-      </c>
-      <c r="D65">
-        <v>1000</v>
-      </c>
-      <c r="E65" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
-        <v>97</v>
-      </c>
       <c r="B66" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C66" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D66">
         <v>1000</v>
       </c>
       <c r="E66" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>55</v>
       </c>
       <c r="B67" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C67" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D67">
         <v>1000</v>
       </c>
       <c r="E67" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>56</v>
       </c>
       <c r="B68" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C68" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D68">
         <v>1000</v>
       </c>
       <c r="E68" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
-        <v>57</v>
-      </c>
-      <c r="B69" t="s">
-        <v>88</v>
-      </c>
-      <c r="C69" t="s">
-        <v>93</v>
-      </c>
-      <c r="D69">
-        <v>1000</v>
-      </c>
-      <c r="E69" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2032,161 +2012,161 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" style="3"/>
     <col min="2" max="2" width="17" style="3" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="19.625" style="3" customWidth="1"/>
     <col min="4" max="16384" width="11" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="B7" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="B9" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="D9" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="E10" s="2"/>
     </row>

</xml_diff>